<commit_message>
added back 4 hrs of 300-level electives...
</commit_message>
<xml_diff>
--- a/data/schedule_2026.xlsx
+++ b/data/schedule_2026.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W96"/>
+  <dimension ref="A1:W98"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1110,7 +1110,7 @@
         <v/>
       </c>
       <c r="D11" t="str">
-        <v/>
+        <v>Full</v>
       </c>
       <c r="E11" t="str">
         <v/>
@@ -3879,25 +3879,25 @@
         <v>FA</v>
       </c>
       <c r="D50" t="str">
-        <v>Full</v>
+        <v>First</v>
       </c>
       <c r="E50" t="str">
         <v>CS</v>
       </c>
       <c r="F50" t="str">
-        <v>336</v>
+        <v>300</v>
       </c>
       <c r="G50" t="str">
         <v>A</v>
       </c>
       <c r="H50" t="str">
-        <v>Victor T. Norman</v>
+        <v>Staff</v>
       </c>
       <c r="I50" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J50" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K50" t="str">
         <v/>
@@ -3906,16 +3906,16 @@
         <v>MWF</v>
       </c>
       <c r="M50" t="str">
-        <v>09:15:00</v>
+        <v>11:00:00</v>
       </c>
       <c r="N50">
         <v>65</v>
       </c>
       <c r="O50" t="str">
-        <v>HH 336</v>
+        <v>SB 382</v>
       </c>
       <c r="P50" t="str">
-        <v>Web Development</v>
+        <v>Applied Machine Learning</v>
       </c>
       <c r="Q50" t="str">
         <v/>
@@ -3927,7 +3927,7 @@
         <v/>
       </c>
       <c r="T50" t="str">
-        <v/>
+        <v>In-Person</v>
       </c>
       <c r="U50" t="str">
         <v/>
@@ -3947,22 +3947,22 @@
         <v/>
       </c>
       <c r="C51" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D51" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="E51" t="str">
         <v>CS</v>
       </c>
       <c r="F51" t="str">
-        <v>338</v>
+        <v>300</v>
       </c>
       <c r="G51" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="H51" t="str">
-        <v>Christopher Wieringa</v>
+        <v>Staff</v>
       </c>
       <c r="I51" t="str">
         <v>2</v>
@@ -3977,7 +3977,7 @@
         <v>MWF</v>
       </c>
       <c r="M51" t="str">
-        <v>08:00:00</v>
+        <v>11:00:00</v>
       </c>
       <c r="N51">
         <v>65</v>
@@ -3986,7 +3986,7 @@
         <v>SB 382</v>
       </c>
       <c r="P51" t="str">
-        <v>System Administration: Infrastructure</v>
+        <v>Applied Machine Learning</v>
       </c>
       <c r="Q51" t="str">
         <v/>
@@ -3998,7 +3998,7 @@
         <v/>
       </c>
       <c r="T51" t="str">
-        <v/>
+        <v>In-Person</v>
       </c>
       <c r="U51" t="str">
         <v/>
@@ -4018,28 +4018,28 @@
         <v/>
       </c>
       <c r="C52" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D52" t="str">
-        <v>Second</v>
+        <v>Full</v>
       </c>
       <c r="E52" t="str">
         <v>CS</v>
       </c>
       <c r="F52" t="str">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G52" t="str">
         <v>A</v>
       </c>
       <c r="H52" t="str">
-        <v>Christopher Wieringa</v>
+        <v>Victor T. Norman</v>
       </c>
       <c r="I52" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J52" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K52" t="str">
         <v/>
@@ -4048,16 +4048,16 @@
         <v>MWF</v>
       </c>
       <c r="M52" t="str">
-        <v>08:00:00</v>
+        <v>09:15:00</v>
       </c>
       <c r="N52">
         <v>65</v>
       </c>
       <c r="O52" t="str">
-        <v>SB 382</v>
+        <v>HH 336</v>
       </c>
       <c r="P52" t="str">
-        <v>System Administration: Cloud Services</v>
+        <v>Web Development</v>
       </c>
       <c r="Q52" t="str">
         <v/>
@@ -4092,19 +4092,19 @@
         <v>SP</v>
       </c>
       <c r="D53" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="E53" t="str">
         <v>CS</v>
       </c>
       <c r="F53" t="str">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="G53" t="str">
         <v>A</v>
       </c>
       <c r="H53" t="str">
-        <v>Eric Araujo</v>
+        <v>Christopher Wieringa</v>
       </c>
       <c r="I53" t="str">
         <v>2</v>
@@ -4119,7 +4119,7 @@
         <v>MWF</v>
       </c>
       <c r="M53" t="str">
-        <v>09:15:00</v>
+        <v>08:00:00</v>
       </c>
       <c r="N53">
         <v>65</v>
@@ -4128,7 +4128,7 @@
         <v>SB 382</v>
       </c>
       <c r="P53" t="str">
-        <v>Database Management Systems</v>
+        <v>System Administration: Infrastructure</v>
       </c>
       <c r="Q53" t="str">
         <v/>
@@ -4160,46 +4160,46 @@
         <v/>
       </c>
       <c r="C54" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D54" t="str">
-        <v>Full</v>
+        <v>Second</v>
       </c>
       <c r="E54" t="str">
         <v>CS</v>
       </c>
       <c r="F54" t="str">
-        <v>364</v>
+        <v>339</v>
       </c>
       <c r="G54" t="str">
         <v>A</v>
       </c>
       <c r="H54" t="str">
-        <v>Brian D Paige, Adam Vedra</v>
+        <v>Christopher Wieringa</v>
       </c>
       <c r="I54" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J54" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K54" t="str">
         <v/>
       </c>
       <c r="L54" t="str">
-        <v>MR</v>
+        <v>MWF</v>
       </c>
       <c r="M54" t="str">
-        <v>19:00:00</v>
+        <v>08:00:00</v>
       </c>
       <c r="N54">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="O54" t="str">
-        <v>SB 372</v>
+        <v>SB 382</v>
       </c>
       <c r="P54" t="str">
-        <v>Computer Security</v>
+        <v>System Administration: Cloud Services</v>
       </c>
       <c r="Q54" t="str">
         <v/>
@@ -4234,19 +4234,19 @@
         <v>SP</v>
       </c>
       <c r="D55" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="E55" t="str">
         <v>CS</v>
       </c>
       <c r="F55" t="str">
-        <v>375</v>
+        <v>354</v>
       </c>
       <c r="G55" t="str">
         <v>A</v>
       </c>
       <c r="H55" t="str">
-        <v>Kenneth C Arnold</v>
+        <v>Eric Araujo</v>
       </c>
       <c r="I55" t="str">
         <v>2</v>
@@ -4261,7 +4261,7 @@
         <v>MWF</v>
       </c>
       <c r="M55" t="str">
-        <v>11:00:00</v>
+        <v>09:15:00</v>
       </c>
       <c r="N55">
         <v>65</v>
@@ -4270,7 +4270,7 @@
         <v>SB 382</v>
       </c>
       <c r="P55" t="str">
-        <v>Artificial Intelligence</v>
+        <v>Database Management Systems</v>
       </c>
       <c r="Q55" t="str">
         <v/>
@@ -4302,46 +4302,46 @@
         <v/>
       </c>
       <c r="C56" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D56" t="str">
-        <v>Second</v>
+        <v>Full</v>
       </c>
       <c r="E56" t="str">
         <v>CS</v>
       </c>
       <c r="F56" t="str">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="G56" t="str">
         <v>A</v>
       </c>
       <c r="H56" t="str">
-        <v>Kenneth C Arnold</v>
+        <v>Brian D Paige, Adam Vedra</v>
       </c>
       <c r="I56" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J56" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K56" t="str">
         <v/>
       </c>
       <c r="L56" t="str">
-        <v>MWF</v>
+        <v>MR</v>
       </c>
       <c r="M56" t="str">
-        <v>11:00:00</v>
+        <v>19:00:00</v>
       </c>
       <c r="N56">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O56" t="str">
-        <v>SB 382</v>
+        <v>SB 372</v>
       </c>
       <c r="P56" t="str">
-        <v>Machine Learning</v>
+        <v>Computer Security</v>
       </c>
       <c r="Q56" t="str">
         <v/>
@@ -4373,46 +4373,46 @@
         <v/>
       </c>
       <c r="C57" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D57" t="str">
-        <v>Full</v>
+        <v>First</v>
       </c>
       <c r="E57" t="str">
         <v>CS</v>
       </c>
       <c r="F57" t="str">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="G57" t="str">
         <v>A</v>
       </c>
       <c r="H57" t="str">
-        <v>Derek C Schuurman</v>
+        <v>Kenneth C Arnold</v>
       </c>
       <c r="I57" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J57" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K57" t="str">
         <v/>
       </c>
       <c r="L57" t="str">
-        <v>R</v>
+        <v>MWF</v>
       </c>
       <c r="M57" t="str">
-        <v>19:00:00</v>
+        <v>11:00:00</v>
       </c>
       <c r="N57">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="O57" t="str">
         <v>SB 382</v>
       </c>
       <c r="P57" t="str">
-        <v>Senior Internship in Computing</v>
+        <v>Artificial Intelligence</v>
       </c>
       <c r="Q57" t="str">
         <v/>
@@ -4447,43 +4447,43 @@
         <v>SP</v>
       </c>
       <c r="D58" t="str">
-        <v>Full</v>
+        <v>Second</v>
       </c>
       <c r="E58" t="str">
         <v>CS</v>
       </c>
       <c r="F58" t="str">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="G58" t="str">
         <v>A</v>
       </c>
       <c r="H58" t="str">
-        <v>Derek C Schuurman</v>
+        <v>Kenneth C Arnold</v>
       </c>
       <c r="I58" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J58" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K58" t="str">
         <v/>
       </c>
       <c r="L58" t="str">
-        <v>R</v>
+        <v>MWF</v>
       </c>
       <c r="M58" t="str">
-        <v>19:00:00</v>
+        <v>11:00:00</v>
       </c>
       <c r="N58">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="O58" t="str">
         <v>SB 382</v>
       </c>
       <c r="P58" t="str">
-        <v>Senior Internship in Computing</v>
+        <v>Machine Learning</v>
       </c>
       <c r="Q58" t="str">
         <v/>
@@ -4515,7 +4515,7 @@
         <v/>
       </c>
       <c r="C59" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D59" t="str">
         <v>Full</v>
@@ -4524,7 +4524,7 @@
         <v>CS</v>
       </c>
       <c r="F59" t="str">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G59" t="str">
         <v>A</v>
@@ -4533,28 +4533,28 @@
         <v>Derek C Schuurman</v>
       </c>
       <c r="I59" t="str">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J59" t="str">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K59" t="str">
         <v/>
       </c>
       <c r="L59" t="str">
-        <v>TR</v>
+        <v>R</v>
       </c>
       <c r="M59" t="str">
-        <v>10:20:00</v>
+        <v>19:00:00</v>
       </c>
       <c r="N59">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O59" t="str">
-        <v>HH 336</v>
+        <v>SB 382</v>
       </c>
       <c r="P59" t="str">
-        <v>Perspectives on Computing</v>
+        <v>Senior Internship in Computing</v>
       </c>
       <c r="Q59" t="str">
         <v/>
@@ -4595,37 +4595,37 @@
         <v>CS</v>
       </c>
       <c r="F60" t="str">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G60" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="H60" t="str">
-        <v>Fernando Pasquini Santos</v>
+        <v>Derek C Schuurman</v>
       </c>
       <c r="I60" t="str">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J60" t="str">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K60" t="str">
         <v/>
       </c>
       <c r="L60" t="str">
-        <v>TR</v>
+        <v>R</v>
       </c>
       <c r="M60" t="str">
-        <v>12:15:00</v>
+        <v>19:00:00</v>
       </c>
       <c r="N60">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O60" t="str">
-        <v>HH 336</v>
+        <v>SB 382</v>
       </c>
       <c r="P60" t="str">
-        <v>Perspectives on Computing</v>
+        <v>Senior Internship in Computing</v>
       </c>
       <c r="Q60" t="str">
         <v/>
@@ -4657,28 +4657,28 @@
         <v/>
       </c>
       <c r="C61" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D61" t="str">
-        <v>First</v>
+        <v>Full</v>
       </c>
       <c r="E61" t="str">
-        <v>DATA</v>
+        <v>CS</v>
       </c>
       <c r="F61" t="str">
-        <v>102</v>
+        <v>384</v>
       </c>
       <c r="G61" t="str">
         <v>A</v>
       </c>
       <c r="H61" t="str">
-        <v>Fernando Pasquini Santos</v>
+        <v>Derek C Schuurman</v>
       </c>
       <c r="I61" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J61" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K61" t="str">
         <v/>
@@ -4687,22 +4687,22 @@
         <v>TR</v>
       </c>
       <c r="M61" t="str">
-        <v>08:00:00</v>
+        <v>10:20:00</v>
       </c>
       <c r="N61">
         <v>100</v>
       </c>
       <c r="O61" t="str">
-        <v>SB 354</v>
+        <v>HH 336</v>
       </c>
       <c r="P61" t="str">
-        <v>Foundations of Data Science and Analytics</v>
+        <v>Perspectives on Computing</v>
       </c>
       <c r="Q61" t="str">
         <v/>
       </c>
       <c r="R61" t="str">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="S61" t="str">
         <v/>
@@ -4728,28 +4728,28 @@
         <v/>
       </c>
       <c r="C62" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D62" t="str">
-        <v>First</v>
+        <v>Full</v>
       </c>
       <c r="E62" t="str">
-        <v>DATA</v>
+        <v>CS</v>
       </c>
       <c r="F62" t="str">
-        <v>102</v>
+        <v>384</v>
       </c>
       <c r="G62" t="str">
         <v>B</v>
       </c>
       <c r="H62" t="str">
-        <v>Cancelled-DATA</v>
+        <v>Fernando Pasquini Santos</v>
       </c>
       <c r="I62" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J62" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K62" t="str">
         <v/>
@@ -4764,16 +4764,16 @@
         <v>100</v>
       </c>
       <c r="O62" t="str">
-        <v>SB 354</v>
+        <v>HH 336</v>
       </c>
       <c r="P62" t="str">
-        <v>Foundations of Data Science and Analytics</v>
+        <v>Perspectives on Computing</v>
       </c>
       <c r="Q62" t="str">
         <v/>
       </c>
       <c r="R62" t="str">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="S62" t="str">
         <v/>
@@ -4799,7 +4799,7 @@
         <v/>
       </c>
       <c r="C63" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D63" t="str">
         <v>First</v>
@@ -4811,10 +4811,10 @@
         <v>102</v>
       </c>
       <c r="G63" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="H63" t="str">
-        <v>Cancelled-DATA</v>
+        <v>Fernando Pasquini Santos</v>
       </c>
       <c r="I63" t="str">
         <v>2</v>
@@ -4829,7 +4829,7 @@
         <v>TR</v>
       </c>
       <c r="M63" t="str">
-        <v>12:15:00</v>
+        <v>08:00:00</v>
       </c>
       <c r="N63">
         <v>100</v>
@@ -4882,7 +4882,7 @@
         <v>102</v>
       </c>
       <c r="G64" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="H64" t="str">
         <v>Cancelled-DATA</v>
@@ -4900,7 +4900,7 @@
         <v>TR</v>
       </c>
       <c r="M64" t="str">
-        <v>14:10:00</v>
+        <v>12:15:00</v>
       </c>
       <c r="N64">
         <v>100</v>
@@ -4953,7 +4953,7 @@
         <v>102</v>
       </c>
       <c r="G65" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="H65" t="str">
         <v>Cancelled-DATA</v>
@@ -4971,7 +4971,7 @@
         <v>TR</v>
       </c>
       <c r="M65" t="str">
-        <v>14:10:00</v>
+        <v>12:15:00</v>
       </c>
       <c r="N65">
         <v>100</v>
@@ -5024,10 +5024,10 @@
         <v>102</v>
       </c>
       <c r="G66" t="str">
-        <v>D</v>
+        <v>C</v>
       </c>
       <c r="H66" t="str">
-        <v>Jim Momeyer</v>
+        <v>Cancelled-DATA</v>
       </c>
       <c r="I66" t="str">
         <v>2</v>
@@ -5042,7 +5042,7 @@
         <v>TR</v>
       </c>
       <c r="M66" t="str">
-        <v>19:00:00</v>
+        <v>14:10:00</v>
       </c>
       <c r="N66">
         <v>100</v>
@@ -5095,10 +5095,10 @@
         <v>102</v>
       </c>
       <c r="G67" t="str">
-        <v>D</v>
+        <v>C</v>
       </c>
       <c r="H67" t="str">
-        <v>Jim Momeyer</v>
+        <v>Cancelled-DATA</v>
       </c>
       <c r="I67" t="str">
         <v>2</v>
@@ -5113,7 +5113,7 @@
         <v>TR</v>
       </c>
       <c r="M67" t="str">
-        <v>19:00:00</v>
+        <v>14:10:00</v>
       </c>
       <c r="N67">
         <v>100</v>
@@ -5157,7 +5157,7 @@
         <v>FA</v>
       </c>
       <c r="D68" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="E68" t="str">
         <v>DATA</v>
@@ -5166,10 +5166,10 @@
         <v>102</v>
       </c>
       <c r="G68" t="str">
-        <v>E</v>
+        <v>D</v>
       </c>
       <c r="H68" t="str">
-        <v>Fernando Pasquini Santos</v>
+        <v>Jim Momeyer</v>
       </c>
       <c r="I68" t="str">
         <v>2</v>
@@ -5184,7 +5184,7 @@
         <v>TR</v>
       </c>
       <c r="M68" t="str">
-        <v>08:00:00</v>
+        <v>19:00:00</v>
       </c>
       <c r="N68">
         <v>100</v>
@@ -5225,10 +5225,10 @@
         <v/>
       </c>
       <c r="C69" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D69" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="E69" t="str">
         <v>DATA</v>
@@ -5237,10 +5237,10 @@
         <v>102</v>
       </c>
       <c r="G69" t="str">
-        <v>F</v>
+        <v>D</v>
       </c>
       <c r="H69" t="str">
-        <v>Cancelled-DATA</v>
+        <v>Jim Momeyer</v>
       </c>
       <c r="I69" t="str">
         <v>2</v>
@@ -5255,7 +5255,7 @@
         <v>TR</v>
       </c>
       <c r="M69" t="str">
-        <v>12:15:00</v>
+        <v>19:00:00</v>
       </c>
       <c r="N69">
         <v>100</v>
@@ -5296,7 +5296,7 @@
         <v/>
       </c>
       <c r="C70" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D70" t="str">
         <v>Second</v>
@@ -5308,10 +5308,10 @@
         <v>102</v>
       </c>
       <c r="G70" t="str">
-        <v>F</v>
+        <v>E</v>
       </c>
       <c r="H70" t="str">
-        <v>Cancelled-DATA</v>
+        <v>Fernando Pasquini Santos</v>
       </c>
       <c r="I70" t="str">
         <v>2</v>
@@ -5326,7 +5326,7 @@
         <v>TR</v>
       </c>
       <c r="M70" t="str">
-        <v>12:15:00</v>
+        <v>08:00:00</v>
       </c>
       <c r="N70">
         <v>100</v>
@@ -5379,7 +5379,7 @@
         <v>102</v>
       </c>
       <c r="G71" t="str">
-        <v>G</v>
+        <v>F</v>
       </c>
       <c r="H71" t="str">
         <v>Cancelled-DATA</v>
@@ -5397,7 +5397,7 @@
         <v>TR</v>
       </c>
       <c r="M71" t="str">
-        <v>14:10:00</v>
+        <v>12:15:00</v>
       </c>
       <c r="N71">
         <v>100</v>
@@ -5450,7 +5450,7 @@
         <v>102</v>
       </c>
       <c r="G72" t="str">
-        <v>G</v>
+        <v>F</v>
       </c>
       <c r="H72" t="str">
         <v>Cancelled-DATA</v>
@@ -5468,7 +5468,7 @@
         <v>TR</v>
       </c>
       <c r="M72" t="str">
-        <v>14:10:00</v>
+        <v>12:15:00</v>
       </c>
       <c r="N72">
         <v>100</v>
@@ -5521,10 +5521,10 @@
         <v>102</v>
       </c>
       <c r="G73" t="str">
-        <v>H</v>
+        <v>G</v>
       </c>
       <c r="H73" t="str">
-        <v>Jim Momeyer</v>
+        <v>Cancelled-DATA</v>
       </c>
       <c r="I73" t="str">
         <v>2</v>
@@ -5539,7 +5539,7 @@
         <v>TR</v>
       </c>
       <c r="M73" t="str">
-        <v>19:00:00</v>
+        <v>14:10:00</v>
       </c>
       <c r="N73">
         <v>100</v>
@@ -5592,10 +5592,10 @@
         <v>102</v>
       </c>
       <c r="G74" t="str">
-        <v>H</v>
+        <v>G</v>
       </c>
       <c r="H74" t="str">
-        <v>Jim Momeyer</v>
+        <v>Cancelled-DATA</v>
       </c>
       <c r="I74" t="str">
         <v>2</v>
@@ -5610,7 +5610,7 @@
         <v>TR</v>
       </c>
       <c r="M74" t="str">
-        <v>19:00:00</v>
+        <v>14:10:00</v>
       </c>
       <c r="N74">
         <v>100</v>
@@ -5643,7 +5643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" xml:space="preserve">
+    <row r="75">
       <c r="A75" t="str">
         <v>Computer Science</v>
       </c>
@@ -5651,10 +5651,10 @@
         <v/>
       </c>
       <c r="C75" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D75" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="E75" t="str">
         <v>DATA</v>
@@ -5663,10 +5663,10 @@
         <v>102</v>
       </c>
       <c r="G75" t="str">
-        <v>A</v>
+        <v>H</v>
       </c>
       <c r="H75" t="str">
-        <v>Staff</v>
+        <v>Jim Momeyer</v>
       </c>
       <c r="I75" t="str">
         <v>2</v>
@@ -5678,13 +5678,13 @@
         <v/>
       </c>
       <c r="L75" t="str">
-        <v>MWF</v>
+        <v>TR</v>
       </c>
       <c r="M75" t="str">
-        <v>09:15:00</v>
+        <v>19:00:00</v>
       </c>
       <c r="N75">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O75" t="str">
         <v>SB 354</v>
@@ -5704,223 +5704,223 @@
       <c r="T75" t="str">
         <v/>
       </c>
-      <c r="U75" t="str" xml:space="preserve">
+      <c r="U75" t="str">
+        <v/>
+      </c>
+      <c r="V75">
+        <v>0</v>
+      </c>
+      <c r="W75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>Computer Science</v>
+      </c>
+      <c r="B76" t="str">
+        <v/>
+      </c>
+      <c r="C76" t="str">
+        <v>SP</v>
+      </c>
+      <c r="D76" t="str">
+        <v>Second</v>
+      </c>
+      <c r="E76" t="str">
+        <v>DATA</v>
+      </c>
+      <c r="F76" t="str">
+        <v>102</v>
+      </c>
+      <c r="G76" t="str">
+        <v>H</v>
+      </c>
+      <c r="H76" t="str">
+        <v>Jim Momeyer</v>
+      </c>
+      <c r="I76" t="str">
+        <v>2</v>
+      </c>
+      <c r="J76" t="str">
+        <v>2</v>
+      </c>
+      <c r="K76" t="str">
+        <v/>
+      </c>
+      <c r="L76" t="str">
+        <v>TR</v>
+      </c>
+      <c r="M76" t="str">
+        <v>19:00:00</v>
+      </c>
+      <c r="N76">
+        <v>100</v>
+      </c>
+      <c r="O76" t="str">
+        <v>SB 354</v>
+      </c>
+      <c r="P76" t="str">
+        <v>Foundations of Data Science and Analytics</v>
+      </c>
+      <c r="Q76" t="str">
+        <v/>
+      </c>
+      <c r="R76" t="str">
+        <v>100</v>
+      </c>
+      <c r="S76" t="str">
+        <v/>
+      </c>
+      <c r="T76" t="str">
+        <v/>
+      </c>
+      <c r="U76" t="str">
+        <v/>
+      </c>
+      <c r="V76">
+        <v>0</v>
+      </c>
+      <c r="W76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" xml:space="preserve">
+      <c r="A77" t="str">
+        <v>Computer Science</v>
+      </c>
+      <c r="B77" t="str">
+        <v/>
+      </c>
+      <c r="C77" t="str">
+        <v>SP</v>
+      </c>
+      <c r="D77" t="str">
+        <v>First</v>
+      </c>
+      <c r="E77" t="str">
+        <v>DATA</v>
+      </c>
+      <c r="F77" t="str">
+        <v>102</v>
+      </c>
+      <c r="G77" t="str">
+        <v>A</v>
+      </c>
+      <c r="H77" t="str">
+        <v>Staff</v>
+      </c>
+      <c r="I77" t="str">
+        <v>2</v>
+      </c>
+      <c r="J77" t="str">
+        <v>2</v>
+      </c>
+      <c r="K77" t="str">
+        <v/>
+      </c>
+      <c r="L77" t="str">
+        <v>MWF</v>
+      </c>
+      <c r="M77" t="str">
+        <v>09:15:00</v>
+      </c>
+      <c r="N77">
+        <v>65</v>
+      </c>
+      <c r="O77" t="str">
+        <v>SB 354</v>
+      </c>
+      <c r="P77" t="str">
+        <v>Foundations of Data Science and Analytics</v>
+      </c>
+      <c r="Q77" t="str">
+        <v/>
+      </c>
+      <c r="R77" t="str">
+        <v>100</v>
+      </c>
+      <c r="S77" t="str">
+        <v/>
+      </c>
+      <c r="T77" t="str">
+        <v/>
+      </c>
+      <c r="U77" t="str" xml:space="preserve">
         <v xml:space="preserve">Monica is busy with ENGR labs all day Thursday.
 Set as on-hold? we may not have the enrollment.</v>
       </c>
-      <c r="V75">
-        <v>0</v>
-      </c>
-      <c r="W75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" xml:space="preserve">
-      <c r="A76" t="str">
+      <c r="V77">
+        <v>0</v>
+      </c>
+      <c r="W77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" xml:space="preserve">
+      <c r="A78" t="str">
         <v>Computer Science</v>
       </c>
-      <c r="B76" t="str">
-        <v/>
-      </c>
-      <c r="C76" t="str">
+      <c r="B78" t="str">
+        <v/>
+      </c>
+      <c r="C78" t="str">
         <v>SP</v>
       </c>
-      <c r="D76" t="str">
+      <c r="D78" t="str">
         <v>Second</v>
       </c>
-      <c r="E76" t="str">
+      <c r="E78" t="str">
         <v>DATA</v>
       </c>
-      <c r="F76" t="str">
+      <c r="F78" t="str">
         <v>102</v>
       </c>
-      <c r="G76" t="str">
+      <c r="G78" t="str">
         <v>E</v>
       </c>
-      <c r="H76" t="str">
+      <c r="H78" t="str">
         <v>Staff</v>
       </c>
-      <c r="I76" t="str">
+      <c r="I78" t="str">
         <v>2</v>
       </c>
-      <c r="J76" t="str">
+      <c r="J78" t="str">
         <v>2</v>
       </c>
-      <c r="K76" t="str">
-        <v/>
-      </c>
-      <c r="L76" t="str">
+      <c r="K78" t="str">
+        <v/>
+      </c>
+      <c r="L78" t="str">
         <v>MWF</v>
       </c>
-      <c r="M76" t="str">
+      <c r="M78" t="str">
         <v>09:15:00</v>
       </c>
-      <c r="N76">
+      <c r="N78">
         <v>65</v>
       </c>
-      <c r="O76" t="str">
+      <c r="O78" t="str">
         <v>SB 354</v>
       </c>
-      <c r="P76" t="str">
+      <c r="P78" t="str">
         <v>Foundations of Data Science and Analytics</v>
       </c>
-      <c r="Q76" t="str">
-        <v/>
-      </c>
-      <c r="R76" t="str">
+      <c r="Q78" t="str">
+        <v/>
+      </c>
+      <c r="R78" t="str">
         <v>100</v>
       </c>
-      <c r="S76" t="str">
-        <v/>
-      </c>
-      <c r="T76" t="str">
-        <v/>
-      </c>
-      <c r="U76" t="str" xml:space="preserve">
+      <c r="S78" t="str">
+        <v/>
+      </c>
+      <c r="T78" t="str">
+        <v/>
+      </c>
+      <c r="U78" t="str" xml:space="preserve">
         <v xml:space="preserve">Monica is busy with ENGR labs all day Thursday.
 Set as on-hold? we may not have the enrollment.</v>
-      </c>
-      <c r="V76">
-        <v>0</v>
-      </c>
-      <c r="W76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="str">
-        <v>Computer Science</v>
-      </c>
-      <c r="B77" t="str">
-        <v/>
-      </c>
-      <c r="C77" t="str">
-        <v>FA</v>
-      </c>
-      <c r="D77" t="str">
-        <v>Full</v>
-      </c>
-      <c r="E77" t="str">
-        <v>DATA</v>
-      </c>
-      <c r="F77" t="str">
-        <v>202</v>
-      </c>
-      <c r="G77" t="str">
-        <v>A</v>
-      </c>
-      <c r="H77" t="str">
-        <v>Fernando Pasquini Santos</v>
-      </c>
-      <c r="I77" t="str">
-        <v>4</v>
-      </c>
-      <c r="J77" t="str">
-        <v>4</v>
-      </c>
-      <c r="K77" t="str">
-        <v/>
-      </c>
-      <c r="L77" t="str">
-        <v>MWF</v>
-      </c>
-      <c r="M77" t="str">
-        <v>08:00:00</v>
-      </c>
-      <c r="N77">
-        <v>65</v>
-      </c>
-      <c r="O77" t="str">
-        <v>SB 382</v>
-      </c>
-      <c r="P77" t="str">
-        <v>Predictive Analytics</v>
-      </c>
-      <c r="Q77" t="str">
-        <v/>
-      </c>
-      <c r="R77" t="str">
-        <v>200</v>
-      </c>
-      <c r="S77" t="str">
-        <v/>
-      </c>
-      <c r="T77" t="str">
-        <v/>
-      </c>
-      <c r="U77" t="str">
-        <v/>
-      </c>
-      <c r="V77">
-        <v>0</v>
-      </c>
-      <c r="W77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="str">
-        <v>Computer Science</v>
-      </c>
-      <c r="B78" t="str">
-        <v/>
-      </c>
-      <c r="C78" t="str">
-        <v>FA</v>
-      </c>
-      <c r="D78" t="str">
-        <v>Full</v>
-      </c>
-      <c r="E78" t="str">
-        <v>DATA</v>
-      </c>
-      <c r="F78" t="str">
-        <v>202</v>
-      </c>
-      <c r="G78" t="str">
-        <v>B</v>
-      </c>
-      <c r="H78" t="str">
-        <v>Fernando Pasquini Santos</v>
-      </c>
-      <c r="I78" t="str">
-        <v>4</v>
-      </c>
-      <c r="J78" t="str">
-        <v>4</v>
-      </c>
-      <c r="K78" t="str">
-        <v/>
-      </c>
-      <c r="L78" t="str">
-        <v>MWF</v>
-      </c>
-      <c r="M78" t="str">
-        <v>09:15:00</v>
-      </c>
-      <c r="N78">
-        <v>65</v>
-      </c>
-      <c r="O78" t="str">
-        <v>SB 382</v>
-      </c>
-      <c r="P78" t="str">
-        <v>Predictive Analytics</v>
-      </c>
-      <c r="Q78" t="str">
-        <v/>
-      </c>
-      <c r="R78" t="str">
-        <v>200</v>
-      </c>
-      <c r="S78" t="str">
-        <v/>
-      </c>
-      <c r="T78" t="str">
-        <v/>
-      </c>
-      <c r="U78" t="str">
-        <v/>
       </c>
       <c r="V78">
         <v>0</v>
@@ -5943,40 +5943,40 @@
         <v>Full</v>
       </c>
       <c r="E79" t="str">
-        <v>HNRS</v>
+        <v>DATA</v>
       </c>
       <c r="F79" t="str">
-        <v>251</v>
+        <v>202</v>
       </c>
       <c r="G79" t="str">
         <v>A</v>
       </c>
       <c r="H79" t="str">
-        <v>Eric Araujo</v>
+        <v>Fernando Pasquini Santos</v>
       </c>
       <c r="I79" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J79" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K79" t="str">
         <v/>
       </c>
       <c r="L79" t="str">
-        <v>TR</v>
+        <v>MWF</v>
       </c>
       <c r="M79" t="str">
-        <v>14:10:00</v>
+        <v>08:00:00</v>
       </c>
       <c r="N79">
         <v>65</v>
       </c>
       <c r="O79" t="str">
-        <v>HL 406C</v>
+        <v>SB 382</v>
       </c>
       <c r="P79" t="str">
-        <v>Agent Modeling</v>
+        <v>Predictive Analytics</v>
       </c>
       <c r="Q79" t="str">
         <v/>
@@ -6002,7 +6002,7 @@
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>Shadow</v>
+        <v>Computer Science</v>
       </c>
       <c r="B80" t="str">
         <v/>
@@ -6011,25 +6011,25 @@
         <v>FA</v>
       </c>
       <c r="D80" t="str">
-        <v>First</v>
+        <v>Full</v>
       </c>
       <c r="E80" t="str">
-        <v>CS</v>
+        <v>DATA</v>
       </c>
       <c r="F80" t="str">
-        <v>300-S</v>
+        <v>202</v>
       </c>
       <c r="G80" t="str">
-        <v>A-S</v>
+        <v>B</v>
       </c>
       <c r="H80" t="str">
-        <v>Shadow-Gold</v>
+        <v>Fernando Pasquini Santos</v>
       </c>
       <c r="I80" t="str">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J80" t="str">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K80" t="str">
         <v/>
@@ -6038,22 +6038,22 @@
         <v>MWF</v>
       </c>
       <c r="M80" t="str">
-        <v>11:00:00</v>
+        <v>09:15:00</v>
       </c>
       <c r="N80">
         <v>65</v>
       </c>
       <c r="O80" t="str">
-        <v>SB 354</v>
+        <v>SB 382</v>
       </c>
       <c r="P80" t="str">
-        <v>Applied Machine Learning</v>
+        <v>Predictive Analytics</v>
       </c>
       <c r="Q80" t="str">
         <v/>
       </c>
       <c r="R80" t="str">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="S80" t="str">
         <v/>
@@ -6073,58 +6073,58 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>Shadow</v>
+        <v>Computer Science</v>
       </c>
       <c r="B81" t="str">
         <v/>
       </c>
       <c r="C81" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D81" t="str">
         <v>Full</v>
       </c>
       <c r="E81" t="str">
-        <v>CS</v>
+        <v>HNRS</v>
       </c>
       <c r="F81" t="str">
-        <v>300-S</v>
+        <v>251</v>
       </c>
       <c r="G81" t="str">
-        <v>A-S</v>
+        <v>A</v>
       </c>
       <c r="H81" t="str">
-        <v>Shadow-Gold</v>
+        <v>Eric Araujo</v>
       </c>
       <c r="I81" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J81" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K81" t="str">
         <v/>
       </c>
       <c r="L81" t="str">
-        <v>MWF</v>
+        <v>TR</v>
       </c>
       <c r="M81" t="str">
-        <v>12:15:00</v>
+        <v>14:10:00</v>
       </c>
       <c r="N81">
         <v>65</v>
       </c>
       <c r="O81" t="str">
-        <v>SB 354</v>
+        <v>HL 406C</v>
       </c>
       <c r="P81" t="str">
-        <v>Applied Machine Learning</v>
+        <v>Agent Modeling</v>
       </c>
       <c r="Q81" t="str">
         <v/>
       </c>
       <c r="R81" t="str">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="S81" t="str">
         <v/>
@@ -6153,7 +6153,7 @@
         <v>FA</v>
       </c>
       <c r="D82" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="E82" t="str">
         <v>CS</v>
@@ -6162,7 +6162,7 @@
         <v>300-S</v>
       </c>
       <c r="G82" t="str">
-        <v>B-S</v>
+        <v>A-S</v>
       </c>
       <c r="H82" t="str">
         <v>Shadow-Gold</v>
@@ -6224,13 +6224,13 @@
         <v>SP</v>
       </c>
       <c r="D83" t="str">
-        <v>First</v>
+        <v>Full</v>
       </c>
       <c r="E83" t="str">
         <v>CS</v>
       </c>
       <c r="F83" t="str">
-        <v>338-S</v>
+        <v>300-S</v>
       </c>
       <c r="G83" t="str">
         <v>A-S</v>
@@ -6251,7 +6251,7 @@
         <v>MWF</v>
       </c>
       <c r="M83" t="str">
-        <v>08:00:00</v>
+        <v>12:15:00</v>
       </c>
       <c r="N83">
         <v>65</v>
@@ -6260,7 +6260,7 @@
         <v>SB 354</v>
       </c>
       <c r="P83" t="str">
-        <v>System Administration: Infrastructure</v>
+        <v>Applied Machine Learning</v>
       </c>
       <c r="Q83" t="str">
         <v/>
@@ -6292,7 +6292,7 @@
         <v/>
       </c>
       <c r="C84" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D84" t="str">
         <v>Second</v>
@@ -6301,10 +6301,10 @@
         <v>CS</v>
       </c>
       <c r="F84" t="str">
-        <v>339-S</v>
+        <v>300-S</v>
       </c>
       <c r="G84" t="str">
-        <v>A-S</v>
+        <v>B-S</v>
       </c>
       <c r="H84" t="str">
         <v>Shadow-Gold</v>
@@ -6322,7 +6322,7 @@
         <v>MWF</v>
       </c>
       <c r="M84" t="str">
-        <v>08:00:00</v>
+        <v>11:00:00</v>
       </c>
       <c r="N84">
         <v>65</v>
@@ -6331,7 +6331,7 @@
         <v>SB 354</v>
       </c>
       <c r="P84" t="str">
-        <v>System Administration: Cloud Services</v>
+        <v>Applied Machine Learning</v>
       </c>
       <c r="Q84" t="str">
         <v/>
@@ -6363,16 +6363,16 @@
         <v/>
       </c>
       <c r="C85" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D85" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="E85" t="str">
         <v>CS</v>
       </c>
       <c r="F85" t="str">
-        <v>374-S</v>
+        <v>338-S</v>
       </c>
       <c r="G85" t="str">
         <v>A-S</v>
@@ -6381,19 +6381,19 @@
         <v>Shadow-Gold</v>
       </c>
       <c r="I85" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J85" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K85" t="str">
         <v/>
       </c>
       <c r="L85" t="str">
-        <v>MW</v>
+        <v>MWF</v>
       </c>
       <c r="M85" t="str">
-        <v>14:45:00</v>
+        <v>08:00:00</v>
       </c>
       <c r="N85">
         <v>65</v>
@@ -6402,7 +6402,7 @@
         <v>SB 354</v>
       </c>
       <c r="P85" t="str">
-        <v>High-Performance Computing</v>
+        <v>System Administration: Infrastructure</v>
       </c>
       <c r="Q85" t="str">
         <v/>
@@ -6437,13 +6437,13 @@
         <v>SP</v>
       </c>
       <c r="D86" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="E86" t="str">
         <v>CS</v>
       </c>
       <c r="F86" t="str">
-        <v>375-S</v>
+        <v>339-S</v>
       </c>
       <c r="G86" t="str">
         <v>A-S</v>
@@ -6464,7 +6464,7 @@
         <v>MWF</v>
       </c>
       <c r="M86" t="str">
-        <v>11:00:00</v>
+        <v>08:00:00</v>
       </c>
       <c r="N86">
         <v>65</v>
@@ -6473,7 +6473,7 @@
         <v>SB 354</v>
       </c>
       <c r="P86" t="str">
-        <v>Artificial Intelligence</v>
+        <v>System Administration: Cloud Services</v>
       </c>
       <c r="Q86" t="str">
         <v/>
@@ -6505,7 +6505,7 @@
         <v/>
       </c>
       <c r="C87" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D87" t="str">
         <v>Second</v>
@@ -6514,28 +6514,28 @@
         <v>CS</v>
       </c>
       <c r="F87" t="str">
-        <v>376-S</v>
+        <v>374-S</v>
       </c>
       <c r="G87" t="str">
-        <v>B-S</v>
+        <v>A-S</v>
       </c>
       <c r="H87" t="str">
         <v>Shadow-Gold</v>
       </c>
       <c r="I87" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J87" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K87" t="str">
         <v/>
       </c>
       <c r="L87" t="str">
-        <v>MWF</v>
+        <v>MW</v>
       </c>
       <c r="M87" t="str">
-        <v>11:00:00</v>
+        <v>14:45:00</v>
       </c>
       <c r="N87">
         <v>65</v>
@@ -6544,7 +6544,7 @@
         <v>SB 354</v>
       </c>
       <c r="P87" t="str">
-        <v>Machine Learning</v>
+        <v>High-Performance Computing</v>
       </c>
       <c r="Q87" t="str">
         <v/>
@@ -6576,22 +6576,22 @@
         <v/>
       </c>
       <c r="C88" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D88" t="str">
-        <v>Full</v>
+        <v>First</v>
       </c>
       <c r="E88" t="str">
-        <v>DATA</v>
+        <v>CS</v>
       </c>
       <c r="F88" t="str">
-        <v>202-S</v>
+        <v>375-S</v>
       </c>
       <c r="G88" t="str">
         <v>A-S</v>
       </c>
       <c r="H88" t="str">
-        <v>Shadow-Maroon</v>
+        <v>Shadow-Gold</v>
       </c>
       <c r="I88" t="str">
         <v>0</v>
@@ -6606,7 +6606,7 @@
         <v>MWF</v>
       </c>
       <c r="M88" t="str">
-        <v>08:00:00</v>
+        <v>11:00:00</v>
       </c>
       <c r="N88">
         <v>65</v>
@@ -6615,13 +6615,13 @@
         <v>SB 354</v>
       </c>
       <c r="P88" t="str">
-        <v>Predictive Analytics</v>
+        <v>Artificial Intelligence</v>
       </c>
       <c r="Q88" t="str">
         <v/>
       </c>
       <c r="R88" t="str">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="S88" t="str">
         <v/>
@@ -6647,22 +6647,22 @@
         <v/>
       </c>
       <c r="C89" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D89" t="str">
-        <v>Full</v>
+        <v>Second</v>
       </c>
       <c r="E89" t="str">
-        <v>DATA</v>
+        <v>CS</v>
       </c>
       <c r="F89" t="str">
-        <v>202-S</v>
+        <v>376-S</v>
       </c>
       <c r="G89" t="str">
         <v>B-S</v>
       </c>
       <c r="H89" t="str">
-        <v>Shadow-Maroon</v>
+        <v>Shadow-Gold</v>
       </c>
       <c r="I89" t="str">
         <v>0</v>
@@ -6677,7 +6677,7 @@
         <v>MWF</v>
       </c>
       <c r="M89" t="str">
-        <v>09:15:00</v>
+        <v>11:00:00</v>
       </c>
       <c r="N89">
         <v>65</v>
@@ -6686,13 +6686,13 @@
         <v>SB 354</v>
       </c>
       <c r="P89" t="str">
-        <v>Predictive Analytics</v>
+        <v>Machine Learning</v>
       </c>
       <c r="Q89" t="str">
         <v/>
       </c>
       <c r="R89" t="str">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="S89" t="str">
         <v/>
@@ -6712,7 +6712,7 @@
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>Computer Science</v>
+        <v>Shadow</v>
       </c>
       <c r="B90" t="str">
         <v/>
@@ -6724,22 +6724,22 @@
         <v>Full</v>
       </c>
       <c r="E90" t="str">
-        <v>CS</v>
+        <v>DATA</v>
       </c>
       <c r="F90" t="str">
-        <v>106</v>
+        <v>202-S</v>
       </c>
       <c r="G90" t="str">
-        <v>A</v>
+        <v>A-S</v>
       </c>
       <c r="H90" t="str">
-        <v>Staff</v>
+        <v>Shadow-Maroon</v>
       </c>
       <c r="I90" t="str">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J90" t="str">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K90" t="str">
         <v/>
@@ -6748,22 +6748,22 @@
         <v>MWF</v>
       </c>
       <c r="M90" t="str">
-        <v>14:45:00</v>
+        <v>08:00:00</v>
       </c>
       <c r="N90">
         <v>65</v>
       </c>
       <c r="O90" t="str">
-        <v>SB 372</v>
+        <v>SB 354</v>
       </c>
       <c r="P90" t="str">
-        <v>Intro to Computing</v>
+        <v>Predictive Analytics</v>
       </c>
       <c r="Q90" t="str">
         <v/>
       </c>
       <c r="R90" t="str">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="S90" t="str">
         <v/>
@@ -6783,7 +6783,7 @@
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>Computer Science</v>
+        <v>Shadow</v>
       </c>
       <c r="B91" t="str">
         <v/>
@@ -6795,46 +6795,46 @@
         <v>Full</v>
       </c>
       <c r="E91" t="str">
-        <v>CS</v>
+        <v>DATA</v>
       </c>
       <c r="F91" t="str">
-        <v>106L</v>
+        <v>202-S</v>
       </c>
       <c r="G91" t="str">
-        <v>A</v>
+        <v>B-S</v>
       </c>
       <c r="H91" t="str">
-        <v>Staff</v>
+        <v>Shadow-Maroon</v>
       </c>
       <c r="I91" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J91" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K91" t="str">
         <v/>
       </c>
       <c r="L91" t="str">
-        <v>R</v>
+        <v>MWF</v>
       </c>
       <c r="M91" t="str">
-        <v>10:20:00</v>
+        <v>09:15:00</v>
       </c>
       <c r="N91">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="O91" t="str">
-        <v>SB 372</v>
+        <v>SB 354</v>
       </c>
       <c r="P91" t="str">
-        <v>Intro to Computing Lab</v>
+        <v>Predictive Analytics</v>
       </c>
       <c r="Q91" t="str">
         <v/>
       </c>
       <c r="R91" t="str">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="S91" t="str">
         <v/>
@@ -6860,7 +6860,7 @@
         <v/>
       </c>
       <c r="C92" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D92" t="str">
         <v>Full</v>
@@ -6869,19 +6869,19 @@
         <v>CS</v>
       </c>
       <c r="F92" t="str">
-        <v>326</v>
+        <v>106</v>
       </c>
       <c r="G92" t="str">
         <v>A</v>
       </c>
       <c r="H92" t="str">
-        <v>Derek C Schuurman</v>
+        <v>Staff</v>
       </c>
       <c r="I92" t="str">
         <v>4</v>
       </c>
       <c r="J92" t="str">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K92" t="str">
         <v/>
@@ -6890,28 +6890,28 @@
         <v>MWF</v>
       </c>
       <c r="M92" t="str">
-        <v>13:30:00</v>
+        <v>14:45:00</v>
       </c>
       <c r="N92">
         <v>65</v>
       </c>
       <c r="O92" t="str">
-        <v>SB 301</v>
+        <v>SB 372</v>
       </c>
       <c r="P92" t="str">
-        <v>Embedded Systems and the Internet of Things</v>
+        <v>Intro to Computing</v>
       </c>
       <c r="Q92" t="str">
         <v/>
       </c>
       <c r="R92" t="str">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="S92" t="str">
         <v/>
       </c>
       <c r="T92" t="str">
-        <v>In-Person</v>
+        <v/>
       </c>
       <c r="U92" t="str">
         <v/>
@@ -6940,7 +6940,7 @@
         <v>CS</v>
       </c>
       <c r="F93" t="str">
-        <v>396</v>
+        <v>106L</v>
       </c>
       <c r="G93" t="str">
         <v>A</v>
@@ -6949,34 +6949,34 @@
         <v>Staff</v>
       </c>
       <c r="I93" t="str">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="J93" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K93" t="str">
         <v/>
       </c>
       <c r="L93" t="str">
-        <v>T</v>
+        <v>R</v>
       </c>
       <c r="M93" t="str">
-        <v>19:00:00</v>
+        <v>10:20:00</v>
       </c>
       <c r="N93">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O93" t="str">
-        <v>SB 382</v>
+        <v>SB 372</v>
       </c>
       <c r="P93" t="str">
-        <v>Senior Project in Computing I</v>
+        <v>Intro to Computing Lab</v>
       </c>
       <c r="Q93" t="str">
         <v/>
       </c>
       <c r="R93" t="str">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="S93" t="str">
         <v/>
@@ -7002,46 +7002,46 @@
         <v/>
       </c>
       <c r="C94" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D94" t="str">
         <v>Full</v>
       </c>
       <c r="E94" t="str">
-        <v>DATA</v>
+        <v>CS</v>
       </c>
       <c r="F94" t="str">
-        <v>396</v>
+        <v>326</v>
       </c>
       <c r="G94" t="str">
         <v>A</v>
       </c>
       <c r="H94" t="str">
-        <v>Staff</v>
+        <v>Derek C Schuurman</v>
       </c>
       <c r="I94" t="str">
-        <v>0.3</v>
+        <v>4</v>
       </c>
       <c r="J94" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K94" t="str">
         <v/>
       </c>
       <c r="L94" t="str">
-        <v>T</v>
+        <v>MWF</v>
       </c>
       <c r="M94" t="str">
-        <v>19:00:00</v>
+        <v>13:30:00</v>
       </c>
       <c r="N94">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="O94" t="str">
-        <v>SB 382</v>
+        <v>SB 301</v>
       </c>
       <c r="P94" t="str">
-        <v>Senior Project in Data Science</v>
+        <v>Embedded Systems and the Internet of Things</v>
       </c>
       <c r="Q94" t="str">
         <v/>
@@ -7053,7 +7053,7 @@
         <v/>
       </c>
       <c r="T94" t="str">
-        <v/>
+        <v>In-Person</v>
       </c>
       <c r="U94" t="str">
         <v/>
@@ -7073,7 +7073,7 @@
         <v/>
       </c>
       <c r="C95" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D95" t="str">
         <v>Full</v>
@@ -7082,7 +7082,7 @@
         <v>CS</v>
       </c>
       <c r="F95" t="str">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G95" t="str">
         <v>A</v>
@@ -7112,7 +7112,7 @@
         <v>SB 382</v>
       </c>
       <c r="P95" t="str">
-        <v>Senior Project in Computing II</v>
+        <v>Senior Project in Computing I</v>
       </c>
       <c r="Q95" t="str">
         <v/>
@@ -7144,7 +7144,7 @@
         <v/>
       </c>
       <c r="C96" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D96" t="str">
         <v>Full</v>
@@ -7153,7 +7153,7 @@
         <v>DATA</v>
       </c>
       <c r="F96" t="str">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G96" t="str">
         <v>A</v>
@@ -7183,7 +7183,7 @@
         <v>SB 382</v>
       </c>
       <c r="P96" t="str">
-        <v>Senior Project in Data Science II</v>
+        <v>Senior Project in Data Science</v>
       </c>
       <c r="Q96" t="str">
         <v/>
@@ -7207,16 +7207,158 @@
         <v>0</v>
       </c>
     </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>Computer Science</v>
+      </c>
+      <c r="B97" t="str">
+        <v/>
+      </c>
+      <c r="C97" t="str">
+        <v>SP</v>
+      </c>
+      <c r="D97" t="str">
+        <v>Full</v>
+      </c>
+      <c r="E97" t="str">
+        <v>CS</v>
+      </c>
+      <c r="F97" t="str">
+        <v>398</v>
+      </c>
+      <c r="G97" t="str">
+        <v>A</v>
+      </c>
+      <c r="H97" t="str">
+        <v>Staff</v>
+      </c>
+      <c r="I97" t="str">
+        <v>0.3</v>
+      </c>
+      <c r="J97" t="str">
+        <v>2</v>
+      </c>
+      <c r="K97" t="str">
+        <v/>
+      </c>
+      <c r="L97" t="str">
+        <v>T</v>
+      </c>
+      <c r="M97" t="str">
+        <v>19:00:00</v>
+      </c>
+      <c r="N97">
+        <v>50</v>
+      </c>
+      <c r="O97" t="str">
+        <v>SB 382</v>
+      </c>
+      <c r="P97" t="str">
+        <v>Senior Project in Computing II</v>
+      </c>
+      <c r="Q97" t="str">
+        <v/>
+      </c>
+      <c r="R97" t="str">
+        <v>300</v>
+      </c>
+      <c r="S97" t="str">
+        <v/>
+      </c>
+      <c r="T97" t="str">
+        <v/>
+      </c>
+      <c r="U97" t="str">
+        <v/>
+      </c>
+      <c r="V97">
+        <v>0</v>
+      </c>
+      <c r="W97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>Computer Science</v>
+      </c>
+      <c r="B98" t="str">
+        <v/>
+      </c>
+      <c r="C98" t="str">
+        <v>SP</v>
+      </c>
+      <c r="D98" t="str">
+        <v>Full</v>
+      </c>
+      <c r="E98" t="str">
+        <v>DATA</v>
+      </c>
+      <c r="F98" t="str">
+        <v>398</v>
+      </c>
+      <c r="G98" t="str">
+        <v>A</v>
+      </c>
+      <c r="H98" t="str">
+        <v>Staff</v>
+      </c>
+      <c r="I98" t="str">
+        <v>0.3</v>
+      </c>
+      <c r="J98" t="str">
+        <v>2</v>
+      </c>
+      <c r="K98" t="str">
+        <v/>
+      </c>
+      <c r="L98" t="str">
+        <v>T</v>
+      </c>
+      <c r="M98" t="str">
+        <v>19:00:00</v>
+      </c>
+      <c r="N98">
+        <v>50</v>
+      </c>
+      <c r="O98" t="str">
+        <v>SB 382</v>
+      </c>
+      <c r="P98" t="str">
+        <v>Senior Project in Data Science II</v>
+      </c>
+      <c r="Q98" t="str">
+        <v/>
+      </c>
+      <c r="R98" t="str">
+        <v>300</v>
+      </c>
+      <c r="S98" t="str">
+        <v/>
+      </c>
+      <c r="T98" t="str">
+        <v/>
+      </c>
+      <c r="U98" t="str">
+        <v/>
+      </c>
+      <c r="V98">
+        <v>0</v>
+      </c>
+      <c r="W98">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:W96"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:W98"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q96"/>
+  <dimension ref="A1:Q98"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7765,7 +7907,10 @@
         <v/>
       </c>
       <c r="J11" t="str">
-        <v/>
+        <v>Full</v>
+      </c>
+      <c r="K11" t="str">
+        <v>-Full</v>
       </c>
       <c r="L11" t="str">
         <v/>
@@ -9808,46 +9953,46 @@
         <v>CS</v>
       </c>
       <c r="C50" t="str">
-        <v>336</v>
+        <v>300</v>
       </c>
       <c r="D50" t="str">
         <v>A</v>
       </c>
       <c r="E50" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F50" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G50" t="str">
         <v>MWF</v>
       </c>
       <c r="H50" t="str">
-        <v>09:15:00 - 10:20:00</v>
+        <v>11:00:00 - 12:05:00</v>
       </c>
       <c r="I50" t="str">
-        <v>HH 336</v>
+        <v>SB 382</v>
       </c>
       <c r="J50" t="str">
-        <v>Full</v>
+        <v>First</v>
       </c>
       <c r="K50" t="str">
-        <v>FA-Full</v>
+        <v>FA-First</v>
       </c>
       <c r="L50">
         <v>65</v>
       </c>
       <c r="M50" t="str">
-        <v>Web Development</v>
+        <v>Applied Machine Learning</v>
       </c>
       <c r="N50" t="str">
-        <v>Victor T. Norman</v>
+        <v>Staff</v>
       </c>
       <c r="O50" t="str">
         <v/>
       </c>
       <c r="P50" t="str">
-        <v/>
+        <v>In-Person</v>
       </c>
       <c r="Q50" t="str">
         <v/>
@@ -9855,16 +10000,16 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B51" t="str">
         <v>CS</v>
       </c>
       <c r="C51" t="str">
-        <v>338</v>
+        <v>300</v>
       </c>
       <c r="D51" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="E51" t="str">
         <v>2</v>
@@ -9876,31 +10021,31 @@
         <v>MWF</v>
       </c>
       <c r="H51" t="str">
-        <v>08:00:00 - 09:05:00</v>
+        <v>11:00:00 - 12:05:00</v>
       </c>
       <c r="I51" t="str">
         <v>SB 382</v>
       </c>
       <c r="J51" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="K51" t="str">
-        <v>SP-First</v>
+        <v>FA-Second</v>
       </c>
       <c r="L51">
         <v>65</v>
       </c>
       <c r="M51" t="str">
-        <v>System Administration: Infrastructure</v>
+        <v>Applied Machine Learning</v>
       </c>
       <c r="N51" t="str">
-        <v>Christopher Wieringa</v>
+        <v>Staff</v>
       </c>
       <c r="O51" t="str">
         <v/>
       </c>
       <c r="P51" t="str">
-        <v/>
+        <v>In-Person</v>
       </c>
       <c r="Q51" t="str">
         <v/>
@@ -9908,46 +10053,46 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B52" t="str">
         <v>CS</v>
       </c>
       <c r="C52" t="str">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D52" t="str">
         <v>A</v>
       </c>
       <c r="E52" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F52" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G52" t="str">
         <v>MWF</v>
       </c>
       <c r="H52" t="str">
-        <v>08:00:00 - 09:05:00</v>
+        <v>09:15:00 - 10:20:00</v>
       </c>
       <c r="I52" t="str">
-        <v>SB 382</v>
+        <v>HH 336</v>
       </c>
       <c r="J52" t="str">
-        <v>Second</v>
+        <v>Full</v>
       </c>
       <c r="K52" t="str">
-        <v>SP-Second</v>
+        <v>FA-Full</v>
       </c>
       <c r="L52">
         <v>65</v>
       </c>
       <c r="M52" t="str">
-        <v>System Administration: Cloud Services</v>
+        <v>Web Development</v>
       </c>
       <c r="N52" t="str">
-        <v>Christopher Wieringa</v>
+        <v>Victor T. Norman</v>
       </c>
       <c r="O52" t="str">
         <v/>
@@ -9967,7 +10112,7 @@
         <v>CS</v>
       </c>
       <c r="C53" t="str">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="D53" t="str">
         <v>A</v>
@@ -9982,25 +10127,25 @@
         <v>MWF</v>
       </c>
       <c r="H53" t="str">
-        <v>09:15:00 - 10:20:00</v>
+        <v>08:00:00 - 09:05:00</v>
       </c>
       <c r="I53" t="str">
         <v>SB 382</v>
       </c>
       <c r="J53" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="K53" t="str">
-        <v>SP-Second</v>
+        <v>SP-First</v>
       </c>
       <c r="L53">
         <v>65</v>
       </c>
       <c r="M53" t="str">
-        <v>Database Management Systems</v>
+        <v>System Administration: Infrastructure</v>
       </c>
       <c r="N53" t="str">
-        <v>Eric Araujo</v>
+        <v>Christopher Wieringa</v>
       </c>
       <c r="O53" t="str">
         <v/>
@@ -10014,46 +10159,46 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B54" t="str">
         <v>CS</v>
       </c>
       <c r="C54" t="str">
-        <v>364</v>
+        <v>339</v>
       </c>
       <c r="D54" t="str">
         <v>A</v>
       </c>
       <c r="E54" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F54" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G54" t="str">
-        <v>MR</v>
+        <v>MWF</v>
       </c>
       <c r="H54" t="str">
-        <v>19:00:00 - 20:40:00</v>
+        <v>08:00:00 - 09:05:00</v>
       </c>
       <c r="I54" t="str">
-        <v>SB 372</v>
+        <v>SB 382</v>
       </c>
       <c r="J54" t="str">
-        <v>Full</v>
+        <v>Second</v>
       </c>
       <c r="K54" t="str">
-        <v>FA-Full</v>
+        <v>SP-Second</v>
       </c>
       <c r="L54">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="M54" t="str">
-        <v>Computer Security</v>
+        <v>System Administration: Cloud Services</v>
       </c>
       <c r="N54" t="str">
-        <v>Brian D Paige, Adam Vedra</v>
+        <v>Christopher Wieringa</v>
       </c>
       <c r="O54" t="str">
         <v/>
@@ -10073,7 +10218,7 @@
         <v>CS</v>
       </c>
       <c r="C55" t="str">
-        <v>375</v>
+        <v>354</v>
       </c>
       <c r="D55" t="str">
         <v>A</v>
@@ -10088,25 +10233,25 @@
         <v>MWF</v>
       </c>
       <c r="H55" t="str">
-        <v>11:00:00 - 12:05:00</v>
+        <v>09:15:00 - 10:20:00</v>
       </c>
       <c r="I55" t="str">
         <v>SB 382</v>
       </c>
       <c r="J55" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="K55" t="str">
-        <v>SP-First</v>
+        <v>SP-Second</v>
       </c>
       <c r="L55">
         <v>65</v>
       </c>
       <c r="M55" t="str">
-        <v>Artificial Intelligence</v>
+        <v>Database Management Systems</v>
       </c>
       <c r="N55" t="str">
-        <v>Kenneth C Arnold</v>
+        <v>Eric Araujo</v>
       </c>
       <c r="O55" t="str">
         <v/>
@@ -10120,46 +10265,46 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B56" t="str">
         <v>CS</v>
       </c>
       <c r="C56" t="str">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="D56" t="str">
         <v>A</v>
       </c>
       <c r="E56" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F56" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G56" t="str">
-        <v>MWF</v>
+        <v>MR</v>
       </c>
       <c r="H56" t="str">
-        <v>11:00:00 - 12:05:00</v>
+        <v>19:00:00 - 20:40:00</v>
       </c>
       <c r="I56" t="str">
-        <v>SB 382</v>
+        <v>SB 372</v>
       </c>
       <c r="J56" t="str">
-        <v>Second</v>
+        <v>Full</v>
       </c>
       <c r="K56" t="str">
-        <v>SP-Second</v>
+        <v>FA-Full</v>
       </c>
       <c r="L56">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="M56" t="str">
-        <v>Machine Learning</v>
+        <v>Computer Security</v>
       </c>
       <c r="N56" t="str">
-        <v>Kenneth C Arnold</v>
+        <v>Brian D Paige, Adam Vedra</v>
       </c>
       <c r="O56" t="str">
         <v/>
@@ -10173,46 +10318,46 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B57" t="str">
         <v>CS</v>
       </c>
       <c r="C57" t="str">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="D57" t="str">
         <v>A</v>
       </c>
       <c r="E57" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F57" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G57" t="str">
-        <v>R</v>
+        <v>MWF</v>
       </c>
       <c r="H57" t="str">
-        <v>19:00:00 - 19:50:00</v>
+        <v>11:00:00 - 12:05:00</v>
       </c>
       <c r="I57" t="str">
         <v>SB 382</v>
       </c>
       <c r="J57" t="str">
-        <v>Full</v>
+        <v>First</v>
       </c>
       <c r="K57" t="str">
-        <v>FA-Full</v>
+        <v>SP-First</v>
       </c>
       <c r="L57">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="M57" t="str">
-        <v>Senior Internship in Computing</v>
+        <v>Artificial Intelligence</v>
       </c>
       <c r="N57" t="str">
-        <v>Derek C Schuurman</v>
+        <v>Kenneth C Arnold</v>
       </c>
       <c r="O57" t="str">
         <v/>
@@ -10232,40 +10377,40 @@
         <v>CS</v>
       </c>
       <c r="C58" t="str">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="D58" t="str">
         <v>A</v>
       </c>
       <c r="E58" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F58" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G58" t="str">
-        <v>R</v>
+        <v>MWF</v>
       </c>
       <c r="H58" t="str">
-        <v>19:00:00 - 19:50:00</v>
+        <v>11:00:00 - 12:05:00</v>
       </c>
       <c r="I58" t="str">
         <v>SB 382</v>
       </c>
       <c r="J58" t="str">
-        <v>Full</v>
+        <v>Second</v>
       </c>
       <c r="K58" t="str">
-        <v>SP-Full</v>
+        <v>SP-Second</v>
       </c>
       <c r="L58">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="M58" t="str">
-        <v>Senior Internship in Computing</v>
+        <v>Machine Learning</v>
       </c>
       <c r="N58" t="str">
-        <v>Derek C Schuurman</v>
+        <v>Kenneth C Arnold</v>
       </c>
       <c r="O58" t="str">
         <v/>
@@ -10279,43 +10424,43 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B59" t="str">
         <v>CS</v>
       </c>
       <c r="C59" t="str">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D59" t="str">
         <v>A</v>
       </c>
       <c r="E59" t="str">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F59" t="str">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G59" t="str">
-        <v>TR</v>
+        <v>R</v>
       </c>
       <c r="H59" t="str">
-        <v>10:20:00 - 12:00:00</v>
+        <v>19:00:00 - 19:50:00</v>
       </c>
       <c r="I59" t="str">
-        <v>HH 336</v>
+        <v>SB 382</v>
       </c>
       <c r="J59" t="str">
         <v>Full</v>
       </c>
       <c r="K59" t="str">
-        <v>SP-Full</v>
+        <v>FA-Full</v>
       </c>
       <c r="L59">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M59" t="str">
-        <v>Perspectives on Computing</v>
+        <v>Senior Internship in Computing</v>
       </c>
       <c r="N59" t="str">
         <v>Derek C Schuurman</v>
@@ -10338,25 +10483,25 @@
         <v>CS</v>
       </c>
       <c r="C60" t="str">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D60" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="E60" t="str">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F60" t="str">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G60" t="str">
-        <v>TR</v>
+        <v>R</v>
       </c>
       <c r="H60" t="str">
-        <v>12:15:00 - 13:55:00</v>
+        <v>19:00:00 - 19:50:00</v>
       </c>
       <c r="I60" t="str">
-        <v>HH 336</v>
+        <v>SB 382</v>
       </c>
       <c r="J60" t="str">
         <v>Full</v>
@@ -10365,13 +10510,13 @@
         <v>SP-Full</v>
       </c>
       <c r="L60">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M60" t="str">
-        <v>Perspectives on Computing</v>
+        <v>Senior Internship in Computing</v>
       </c>
       <c r="N60" t="str">
-        <v>Fernando Pasquini Santos</v>
+        <v>Derek C Schuurman</v>
       </c>
       <c r="O60" t="str">
         <v/>
@@ -10385,46 +10530,46 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B61" t="str">
-        <v>DATA</v>
+        <v>CS</v>
       </c>
       <c r="C61" t="str">
-        <v>102</v>
+        <v>384</v>
       </c>
       <c r="D61" t="str">
         <v>A</v>
       </c>
       <c r="E61" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F61" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G61" t="str">
         <v>TR</v>
       </c>
       <c r="H61" t="str">
-        <v>08:00:00 - 09:40:00</v>
+        <v>10:20:00 - 12:00:00</v>
       </c>
       <c r="I61" t="str">
-        <v>SB 354</v>
+        <v>HH 336</v>
       </c>
       <c r="J61" t="str">
-        <v>First</v>
+        <v>Full</v>
       </c>
       <c r="K61" t="str">
-        <v>FA-First</v>
+        <v>SP-Full</v>
       </c>
       <c r="L61">
         <v>100</v>
       </c>
       <c r="M61" t="str">
-        <v>Foundations of Data Science and Analytics</v>
+        <v>Perspectives on Computing</v>
       </c>
       <c r="N61" t="str">
-        <v>Fernando Pasquini Santos</v>
+        <v>Derek C Schuurman</v>
       </c>
       <c r="O61" t="str">
         <v/>
@@ -10438,22 +10583,22 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B62" t="str">
-        <v>DATA</v>
+        <v>CS</v>
       </c>
       <c r="C62" t="str">
-        <v>102</v>
+        <v>384</v>
       </c>
       <c r="D62" t="str">
         <v>B</v>
       </c>
       <c r="E62" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F62" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G62" t="str">
         <v>TR</v>
@@ -10462,22 +10607,22 @@
         <v>12:15:00 - 13:55:00</v>
       </c>
       <c r="I62" t="str">
-        <v>SB 354</v>
+        <v>HH 336</v>
       </c>
       <c r="J62" t="str">
-        <v>First</v>
+        <v>Full</v>
       </c>
       <c r="K62" t="str">
-        <v>FA-First</v>
+        <v>SP-Full</v>
       </c>
       <c r="L62">
         <v>100</v>
       </c>
       <c r="M62" t="str">
-        <v>Foundations of Data Science and Analytics</v>
+        <v>Perspectives on Computing</v>
       </c>
       <c r="N62" t="str">
-        <v>Cancelled-DATA</v>
+        <v>Fernando Pasquini Santos</v>
       </c>
       <c r="O62" t="str">
         <v/>
@@ -10491,7 +10636,7 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B63" t="str">
         <v>DATA</v>
@@ -10500,7 +10645,7 @@
         <v>102</v>
       </c>
       <c r="D63" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="E63" t="str">
         <v>2</v>
@@ -10512,7 +10657,7 @@
         <v>TR</v>
       </c>
       <c r="H63" t="str">
-        <v>12:15:00 - 13:55:00</v>
+        <v>08:00:00 - 09:40:00</v>
       </c>
       <c r="I63" t="str">
         <v>SB 354</v>
@@ -10521,7 +10666,7 @@
         <v>First</v>
       </c>
       <c r="K63" t="str">
-        <v>SP-First</v>
+        <v>FA-First</v>
       </c>
       <c r="L63">
         <v>100</v>
@@ -10530,7 +10675,7 @@
         <v>Foundations of Data Science and Analytics</v>
       </c>
       <c r="N63" t="str">
-        <v>Cancelled-DATA</v>
+        <v>Fernando Pasquini Santos</v>
       </c>
       <c r="O63" t="str">
         <v/>
@@ -10553,7 +10698,7 @@
         <v>102</v>
       </c>
       <c r="D64" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="E64" t="str">
         <v>2</v>
@@ -10565,7 +10710,7 @@
         <v>TR</v>
       </c>
       <c r="H64" t="str">
-        <v>14:10:00 - 15:50:00</v>
+        <v>12:15:00 - 13:55:00</v>
       </c>
       <c r="I64" t="str">
         <v>SB 354</v>
@@ -10606,7 +10751,7 @@
         <v>102</v>
       </c>
       <c r="D65" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="E65" t="str">
         <v>2</v>
@@ -10618,7 +10763,7 @@
         <v>TR</v>
       </c>
       <c r="H65" t="str">
-        <v>14:10:00 - 15:50:00</v>
+        <v>12:15:00 - 13:55:00</v>
       </c>
       <c r="I65" t="str">
         <v>SB 354</v>
@@ -10659,7 +10804,7 @@
         <v>102</v>
       </c>
       <c r="D66" t="str">
-        <v>D</v>
+        <v>C</v>
       </c>
       <c r="E66" t="str">
         <v>2</v>
@@ -10671,7 +10816,7 @@
         <v>TR</v>
       </c>
       <c r="H66" t="str">
-        <v>19:00:00 - 20:40:00</v>
+        <v>14:10:00 - 15:50:00</v>
       </c>
       <c r="I66" t="str">
         <v>SB 354</v>
@@ -10689,7 +10834,7 @@
         <v>Foundations of Data Science and Analytics</v>
       </c>
       <c r="N66" t="str">
-        <v>Jim Momeyer</v>
+        <v>Cancelled-DATA</v>
       </c>
       <c r="O66" t="str">
         <v/>
@@ -10712,7 +10857,7 @@
         <v>102</v>
       </c>
       <c r="D67" t="str">
-        <v>D</v>
+        <v>C</v>
       </c>
       <c r="E67" t="str">
         <v>2</v>
@@ -10724,7 +10869,7 @@
         <v>TR</v>
       </c>
       <c r="H67" t="str">
-        <v>19:00:00 - 20:40:00</v>
+        <v>14:10:00 - 15:50:00</v>
       </c>
       <c r="I67" t="str">
         <v>SB 354</v>
@@ -10742,7 +10887,7 @@
         <v>Foundations of Data Science and Analytics</v>
       </c>
       <c r="N67" t="str">
-        <v>Jim Momeyer</v>
+        <v>Cancelled-DATA</v>
       </c>
       <c r="O67" t="str">
         <v/>
@@ -10765,7 +10910,7 @@
         <v>102</v>
       </c>
       <c r="D68" t="str">
-        <v>E</v>
+        <v>D</v>
       </c>
       <c r="E68" t="str">
         <v>2</v>
@@ -10777,16 +10922,16 @@
         <v>TR</v>
       </c>
       <c r="H68" t="str">
-        <v>08:00:00 - 09:40:00</v>
+        <v>19:00:00 - 20:40:00</v>
       </c>
       <c r="I68" t="str">
         <v>SB 354</v>
       </c>
       <c r="J68" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="K68" t="str">
-        <v>FA-Second</v>
+        <v>FA-First</v>
       </c>
       <c r="L68">
         <v>100</v>
@@ -10795,7 +10940,7 @@
         <v>Foundations of Data Science and Analytics</v>
       </c>
       <c r="N68" t="str">
-        <v>Fernando Pasquini Santos</v>
+        <v>Jim Momeyer</v>
       </c>
       <c r="O68" t="str">
         <v/>
@@ -10809,7 +10954,7 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B69" t="str">
         <v>DATA</v>
@@ -10818,7 +10963,7 @@
         <v>102</v>
       </c>
       <c r="D69" t="str">
-        <v>F</v>
+        <v>D</v>
       </c>
       <c r="E69" t="str">
         <v>2</v>
@@ -10830,16 +10975,16 @@
         <v>TR</v>
       </c>
       <c r="H69" t="str">
-        <v>12:15:00 - 13:55:00</v>
+        <v>19:00:00 - 20:40:00</v>
       </c>
       <c r="I69" t="str">
         <v>SB 354</v>
       </c>
       <c r="J69" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="K69" t="str">
-        <v>FA-Second</v>
+        <v>SP-First</v>
       </c>
       <c r="L69">
         <v>100</v>
@@ -10848,7 +10993,7 @@
         <v>Foundations of Data Science and Analytics</v>
       </c>
       <c r="N69" t="str">
-        <v>Cancelled-DATA</v>
+        <v>Jim Momeyer</v>
       </c>
       <c r="O69" t="str">
         <v/>
@@ -10862,7 +11007,7 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B70" t="str">
         <v>DATA</v>
@@ -10871,7 +11016,7 @@
         <v>102</v>
       </c>
       <c r="D70" t="str">
-        <v>F</v>
+        <v>E</v>
       </c>
       <c r="E70" t="str">
         <v>2</v>
@@ -10883,7 +11028,7 @@
         <v>TR</v>
       </c>
       <c r="H70" t="str">
-        <v>12:15:00 - 13:55:00</v>
+        <v>08:00:00 - 09:40:00</v>
       </c>
       <c r="I70" t="str">
         <v>SB 354</v>
@@ -10892,7 +11037,7 @@
         <v>Second</v>
       </c>
       <c r="K70" t="str">
-        <v>SP-Second</v>
+        <v>FA-Second</v>
       </c>
       <c r="L70">
         <v>100</v>
@@ -10901,7 +11046,7 @@
         <v>Foundations of Data Science and Analytics</v>
       </c>
       <c r="N70" t="str">
-        <v>Cancelled-DATA</v>
+        <v>Fernando Pasquini Santos</v>
       </c>
       <c r="O70" t="str">
         <v/>
@@ -10924,7 +11069,7 @@
         <v>102</v>
       </c>
       <c r="D71" t="str">
-        <v>G</v>
+        <v>F</v>
       </c>
       <c r="E71" t="str">
         <v>2</v>
@@ -10936,7 +11081,7 @@
         <v>TR</v>
       </c>
       <c r="H71" t="str">
-        <v>14:10:00 - 15:50:00</v>
+        <v>12:15:00 - 13:55:00</v>
       </c>
       <c r="I71" t="str">
         <v>SB 354</v>
@@ -10977,7 +11122,7 @@
         <v>102</v>
       </c>
       <c r="D72" t="str">
-        <v>G</v>
+        <v>F</v>
       </c>
       <c r="E72" t="str">
         <v>2</v>
@@ -10989,7 +11134,7 @@
         <v>TR</v>
       </c>
       <c r="H72" t="str">
-        <v>14:10:00 - 15:50:00</v>
+        <v>12:15:00 - 13:55:00</v>
       </c>
       <c r="I72" t="str">
         <v>SB 354</v>
@@ -11030,7 +11175,7 @@
         <v>102</v>
       </c>
       <c r="D73" t="str">
-        <v>H</v>
+        <v>G</v>
       </c>
       <c r="E73" t="str">
         <v>2</v>
@@ -11042,7 +11187,7 @@
         <v>TR</v>
       </c>
       <c r="H73" t="str">
-        <v>19:00:00 - 20:40:00</v>
+        <v>14:10:00 - 15:50:00</v>
       </c>
       <c r="I73" t="str">
         <v>SB 354</v>
@@ -11060,7 +11205,7 @@
         <v>Foundations of Data Science and Analytics</v>
       </c>
       <c r="N73" t="str">
-        <v>Jim Momeyer</v>
+        <v>Cancelled-DATA</v>
       </c>
       <c r="O73" t="str">
         <v/>
@@ -11083,7 +11228,7 @@
         <v>102</v>
       </c>
       <c r="D74" t="str">
-        <v>H</v>
+        <v>G</v>
       </c>
       <c r="E74" t="str">
         <v>2</v>
@@ -11095,7 +11240,7 @@
         <v>TR</v>
       </c>
       <c r="H74" t="str">
-        <v>19:00:00 - 20:40:00</v>
+        <v>14:10:00 - 15:50:00</v>
       </c>
       <c r="I74" t="str">
         <v>SB 354</v>
@@ -11113,7 +11258,7 @@
         <v>Foundations of Data Science and Analytics</v>
       </c>
       <c r="N74" t="str">
-        <v>Jim Momeyer</v>
+        <v>Cancelled-DATA</v>
       </c>
       <c r="O74" t="str">
         <v/>
@@ -11125,9 +11270,9 @@
         <v/>
       </c>
     </row>
-    <row r="75" xml:space="preserve">
+    <row r="75">
       <c r="A75" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B75" t="str">
         <v>DATA</v>
@@ -11136,7 +11281,7 @@
         <v>102</v>
       </c>
       <c r="D75" t="str">
-        <v>A</v>
+        <v>H</v>
       </c>
       <c r="E75" t="str">
         <v>2</v>
@@ -11145,198 +11290,198 @@
         <v>2</v>
       </c>
       <c r="G75" t="str">
-        <v>MWF</v>
+        <v>TR</v>
       </c>
       <c r="H75" t="str">
-        <v>09:15:00 - 10:20:00</v>
+        <v>19:00:00 - 20:40:00</v>
       </c>
       <c r="I75" t="str">
         <v>SB 354</v>
       </c>
       <c r="J75" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="K75" t="str">
-        <v>SP-First</v>
+        <v>FA-Second</v>
       </c>
       <c r="L75">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="M75" t="str">
         <v>Foundations of Data Science and Analytics</v>
       </c>
       <c r="N75" t="str">
+        <v>Jim Momeyer</v>
+      </c>
+      <c r="O75" t="str">
+        <v/>
+      </c>
+      <c r="P75" t="str">
+        <v/>
+      </c>
+      <c r="Q75" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>SP</v>
+      </c>
+      <c r="B76" t="str">
+        <v>DATA</v>
+      </c>
+      <c r="C76" t="str">
+        <v>102</v>
+      </c>
+      <c r="D76" t="str">
+        <v>H</v>
+      </c>
+      <c r="E76" t="str">
+        <v>2</v>
+      </c>
+      <c r="F76" t="str">
+        <v>2</v>
+      </c>
+      <c r="G76" t="str">
+        <v>TR</v>
+      </c>
+      <c r="H76" t="str">
+        <v>19:00:00 - 20:40:00</v>
+      </c>
+      <c r="I76" t="str">
+        <v>SB 354</v>
+      </c>
+      <c r="J76" t="str">
+        <v>Second</v>
+      </c>
+      <c r="K76" t="str">
+        <v>SP-Second</v>
+      </c>
+      <c r="L76">
+        <v>100</v>
+      </c>
+      <c r="M76" t="str">
+        <v>Foundations of Data Science and Analytics</v>
+      </c>
+      <c r="N76" t="str">
+        <v>Jim Momeyer</v>
+      </c>
+      <c r="O76" t="str">
+        <v/>
+      </c>
+      <c r="P76" t="str">
+        <v/>
+      </c>
+      <c r="Q76" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="77" xml:space="preserve">
+      <c r="A77" t="str">
+        <v>SP</v>
+      </c>
+      <c r="B77" t="str">
+        <v>DATA</v>
+      </c>
+      <c r="C77" t="str">
+        <v>102</v>
+      </c>
+      <c r="D77" t="str">
+        <v>A</v>
+      </c>
+      <c r="E77" t="str">
+        <v>2</v>
+      </c>
+      <c r="F77" t="str">
+        <v>2</v>
+      </c>
+      <c r="G77" t="str">
+        <v>MWF</v>
+      </c>
+      <c r="H77" t="str">
+        <v>09:15:00 - 10:20:00</v>
+      </c>
+      <c r="I77" t="str">
+        <v>SB 354</v>
+      </c>
+      <c r="J77" t="str">
+        <v>First</v>
+      </c>
+      <c r="K77" t="str">
+        <v>SP-First</v>
+      </c>
+      <c r="L77">
+        <v>65</v>
+      </c>
+      <c r="M77" t="str">
+        <v>Foundations of Data Science and Analytics</v>
+      </c>
+      <c r="N77" t="str">
         <v>Staff</v>
       </c>
-      <c r="O75" t="str">
-        <v/>
-      </c>
-      <c r="P75" t="str">
-        <v/>
-      </c>
-      <c r="Q75" t="str" xml:space="preserve">
+      <c r="O77" t="str">
+        <v/>
+      </c>
+      <c r="P77" t="str">
+        <v/>
+      </c>
+      <c r="Q77" t="str" xml:space="preserve">
         <v xml:space="preserve">Monica is busy with ENGR labs all day Thursday.
 Set as on-hold? we may not have the enrollment.</v>
       </c>
     </row>
-    <row r="76" xml:space="preserve">
-      <c r="A76" t="str">
+    <row r="78" xml:space="preserve">
+      <c r="A78" t="str">
         <v>SP</v>
       </c>
-      <c r="B76" t="str">
+      <c r="B78" t="str">
         <v>DATA</v>
       </c>
-      <c r="C76" t="str">
+      <c r="C78" t="str">
         <v>102</v>
       </c>
-      <c r="D76" t="str">
+      <c r="D78" t="str">
         <v>E</v>
       </c>
-      <c r="E76" t="str">
+      <c r="E78" t="str">
         <v>2</v>
       </c>
-      <c r="F76" t="str">
+      <c r="F78" t="str">
         <v>2</v>
       </c>
-      <c r="G76" t="str">
+      <c r="G78" t="str">
         <v>MWF</v>
       </c>
-      <c r="H76" t="str">
+      <c r="H78" t="str">
         <v>09:15:00 - 10:20:00</v>
       </c>
-      <c r="I76" t="str">
+      <c r="I78" t="str">
         <v>SB 354</v>
       </c>
-      <c r="J76" t="str">
+      <c r="J78" t="str">
         <v>Second</v>
       </c>
-      <c r="K76" t="str">
+      <c r="K78" t="str">
         <v>SP-Second</v>
       </c>
-      <c r="L76">
+      <c r="L78">
         <v>65</v>
       </c>
-      <c r="M76" t="str">
+      <c r="M78" t="str">
         <v>Foundations of Data Science and Analytics</v>
       </c>
-      <c r="N76" t="str">
+      <c r="N78" t="str">
         <v>Staff</v>
       </c>
-      <c r="O76" t="str">
-        <v/>
-      </c>
-      <c r="P76" t="str">
-        <v/>
-      </c>
-      <c r="Q76" t="str" xml:space="preserve">
+      <c r="O78" t="str">
+        <v/>
+      </c>
+      <c r="P78" t="str">
+        <v/>
+      </c>
+      <c r="Q78" t="str" xml:space="preserve">
         <v xml:space="preserve">Monica is busy with ENGR labs all day Thursday.
 Set as on-hold? we may not have the enrollment.</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="str">
-        <v>FA</v>
-      </c>
-      <c r="B77" t="str">
-        <v>DATA</v>
-      </c>
-      <c r="C77" t="str">
-        <v>202</v>
-      </c>
-      <c r="D77" t="str">
-        <v>A</v>
-      </c>
-      <c r="E77" t="str">
-        <v>4</v>
-      </c>
-      <c r="F77" t="str">
-        <v>4</v>
-      </c>
-      <c r="G77" t="str">
-        <v>MWF</v>
-      </c>
-      <c r="H77" t="str">
-        <v>08:00:00 - 09:05:00</v>
-      </c>
-      <c r="I77" t="str">
-        <v>SB 382</v>
-      </c>
-      <c r="J77" t="str">
-        <v>Full</v>
-      </c>
-      <c r="K77" t="str">
-        <v>FA-Full</v>
-      </c>
-      <c r="L77">
-        <v>65</v>
-      </c>
-      <c r="M77" t="str">
-        <v>Predictive Analytics</v>
-      </c>
-      <c r="N77" t="str">
-        <v>Fernando Pasquini Santos</v>
-      </c>
-      <c r="O77" t="str">
-        <v/>
-      </c>
-      <c r="P77" t="str">
-        <v/>
-      </c>
-      <c r="Q77" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="str">
-        <v>FA</v>
-      </c>
-      <c r="B78" t="str">
-        <v>DATA</v>
-      </c>
-      <c r="C78" t="str">
-        <v>202</v>
-      </c>
-      <c r="D78" t="str">
-        <v>B</v>
-      </c>
-      <c r="E78" t="str">
-        <v>4</v>
-      </c>
-      <c r="F78" t="str">
-        <v>4</v>
-      </c>
-      <c r="G78" t="str">
-        <v>MWF</v>
-      </c>
-      <c r="H78" t="str">
-        <v>09:15:00 - 10:20:00</v>
-      </c>
-      <c r="I78" t="str">
-        <v>SB 382</v>
-      </c>
-      <c r="J78" t="str">
-        <v>Full</v>
-      </c>
-      <c r="K78" t="str">
-        <v>FA-Full</v>
-      </c>
-      <c r="L78">
-        <v>65</v>
-      </c>
-      <c r="M78" t="str">
-        <v>Predictive Analytics</v>
-      </c>
-      <c r="N78" t="str">
-        <v>Fernando Pasquini Santos</v>
-      </c>
-      <c r="O78" t="str">
-        <v/>
-      </c>
-      <c r="P78" t="str">
-        <v/>
-      </c>
-      <c r="Q78" t="str">
-        <v/>
       </c>
     </row>
     <row r="79">
@@ -11344,28 +11489,28 @@
         <v>FA</v>
       </c>
       <c r="B79" t="str">
-        <v>HNRS</v>
+        <v>DATA</v>
       </c>
       <c r="C79" t="str">
-        <v>251</v>
+        <v>202</v>
       </c>
       <c r="D79" t="str">
         <v>A</v>
       </c>
       <c r="E79" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F79" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G79" t="str">
-        <v>TR</v>
+        <v>MWF</v>
       </c>
       <c r="H79" t="str">
-        <v>14:10:00 - 15:15:00</v>
+        <v>08:00:00 - 09:05:00</v>
       </c>
       <c r="I79" t="str">
-        <v>HL 406C</v>
+        <v>SB 382</v>
       </c>
       <c r="J79" t="str">
         <v>Full</v>
@@ -11377,10 +11522,10 @@
         <v>65</v>
       </c>
       <c r="M79" t="str">
-        <v>Agent Modeling</v>
+        <v>Predictive Analytics</v>
       </c>
       <c r="N79" t="str">
-        <v>Eric Araujo</v>
+        <v>Fernando Pasquini Santos</v>
       </c>
       <c r="O79" t="str">
         <v/>
@@ -11397,43 +11542,43 @@
         <v>FA</v>
       </c>
       <c r="B80" t="str">
-        <v>CS</v>
+        <v>DATA</v>
       </c>
       <c r="C80" t="str">
-        <v>300-S</v>
+        <v>202</v>
       </c>
       <c r="D80" t="str">
-        <v>A-S</v>
+        <v>B</v>
       </c>
       <c r="E80" t="str">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F80" t="str">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G80" t="str">
         <v>MWF</v>
       </c>
       <c r="H80" t="str">
-        <v>11:00:00 - 12:05:00</v>
+        <v>09:15:00 - 10:20:00</v>
       </c>
       <c r="I80" t="str">
-        <v>SB 354</v>
+        <v>SB 382</v>
       </c>
       <c r="J80" t="str">
-        <v>First</v>
+        <v>Full</v>
       </c>
       <c r="K80" t="str">
-        <v>FA-First</v>
+        <v>FA-Full</v>
       </c>
       <c r="L80">
         <v>65</v>
       </c>
       <c r="M80" t="str">
-        <v>Applied Machine Learning</v>
+        <v>Predictive Analytics</v>
       </c>
       <c r="N80" t="str">
-        <v>Shadow-Gold</v>
+        <v>Fernando Pasquini Santos</v>
       </c>
       <c r="O80" t="str">
         <v/>
@@ -11447,46 +11592,46 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B81" t="str">
-        <v>CS</v>
+        <v>HNRS</v>
       </c>
       <c r="C81" t="str">
-        <v>300-S</v>
+        <v>251</v>
       </c>
       <c r="D81" t="str">
-        <v>A-S</v>
+        <v>A</v>
       </c>
       <c r="E81" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F81" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G81" t="str">
-        <v>MWF</v>
+        <v>TR</v>
       </c>
       <c r="H81" t="str">
-        <v>12:15:00 - 13:20:00</v>
+        <v>14:10:00 - 15:15:00</v>
       </c>
       <c r="I81" t="str">
-        <v>SB 354</v>
+        <v>HL 406C</v>
       </c>
       <c r="J81" t="str">
         <v>Full</v>
       </c>
       <c r="K81" t="str">
-        <v>SP-Full</v>
+        <v>FA-Full</v>
       </c>
       <c r="L81">
         <v>65</v>
       </c>
       <c r="M81" t="str">
-        <v>Applied Machine Learning</v>
+        <v>Agent Modeling</v>
       </c>
       <c r="N81" t="str">
-        <v>Shadow-Gold</v>
+        <v>Eric Araujo</v>
       </c>
       <c r="O81" t="str">
         <v/>
@@ -11509,7 +11654,7 @@
         <v>300-S</v>
       </c>
       <c r="D82" t="str">
-        <v>B-S</v>
+        <v>A-S</v>
       </c>
       <c r="E82" t="str">
         <v>0</v>
@@ -11527,10 +11672,10 @@
         <v>SB 354</v>
       </c>
       <c r="J82" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="K82" t="str">
-        <v>FA-Second</v>
+        <v>FA-First</v>
       </c>
       <c r="L82">
         <v>65</v>
@@ -11559,7 +11704,7 @@
         <v>CS</v>
       </c>
       <c r="C83" t="str">
-        <v>338-S</v>
+        <v>300-S</v>
       </c>
       <c r="D83" t="str">
         <v>A-S</v>
@@ -11574,22 +11719,22 @@
         <v>MWF</v>
       </c>
       <c r="H83" t="str">
-        <v>08:00:00 - 09:05:00</v>
+        <v>12:15:00 - 13:20:00</v>
       </c>
       <c r="I83" t="str">
         <v>SB 354</v>
       </c>
       <c r="J83" t="str">
-        <v>First</v>
+        <v>Full</v>
       </c>
       <c r="K83" t="str">
-        <v>SP-First</v>
+        <v>SP-Full</v>
       </c>
       <c r="L83">
         <v>65</v>
       </c>
       <c r="M83" t="str">
-        <v>System Administration: Infrastructure</v>
+        <v>Applied Machine Learning</v>
       </c>
       <c r="N83" t="str">
         <v>Shadow-Gold</v>
@@ -11606,16 +11751,16 @@
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B84" t="str">
         <v>CS</v>
       </c>
       <c r="C84" t="str">
-        <v>339-S</v>
+        <v>300-S</v>
       </c>
       <c r="D84" t="str">
-        <v>A-S</v>
+        <v>B-S</v>
       </c>
       <c r="E84" t="str">
         <v>0</v>
@@ -11627,7 +11772,7 @@
         <v>MWF</v>
       </c>
       <c r="H84" t="str">
-        <v>08:00:00 - 09:05:00</v>
+        <v>11:00:00 - 12:05:00</v>
       </c>
       <c r="I84" t="str">
         <v>SB 354</v>
@@ -11636,13 +11781,13 @@
         <v>Second</v>
       </c>
       <c r="K84" t="str">
-        <v>SP-Second</v>
+        <v>FA-Second</v>
       </c>
       <c r="L84">
         <v>65</v>
       </c>
       <c r="M84" t="str">
-        <v>System Administration: Cloud Services</v>
+        <v>Applied Machine Learning</v>
       </c>
       <c r="N84" t="str">
         <v>Shadow-Gold</v>
@@ -11659,43 +11804,43 @@
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B85" t="str">
         <v>CS</v>
       </c>
       <c r="C85" t="str">
-        <v>374-S</v>
+        <v>338-S</v>
       </c>
       <c r="D85" t="str">
         <v>A-S</v>
       </c>
       <c r="E85" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F85" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G85" t="str">
-        <v>MW</v>
+        <v>MWF</v>
       </c>
       <c r="H85" t="str">
-        <v>14:45:00 - 15:50:00</v>
+        <v>08:00:00 - 09:05:00</v>
       </c>
       <c r="I85" t="str">
         <v>SB 354</v>
       </c>
       <c r="J85" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="K85" t="str">
-        <v>FA-Second</v>
+        <v>SP-First</v>
       </c>
       <c r="L85">
         <v>65</v>
       </c>
       <c r="M85" t="str">
-        <v>High-Performance Computing</v>
+        <v>System Administration: Infrastructure</v>
       </c>
       <c r="N85" t="str">
         <v>Shadow-Gold</v>
@@ -11718,7 +11863,7 @@
         <v>CS</v>
       </c>
       <c r="C86" t="str">
-        <v>375-S</v>
+        <v>339-S</v>
       </c>
       <c r="D86" t="str">
         <v>A-S</v>
@@ -11733,22 +11878,22 @@
         <v>MWF</v>
       </c>
       <c r="H86" t="str">
-        <v>11:00:00 - 12:05:00</v>
+        <v>08:00:00 - 09:05:00</v>
       </c>
       <c r="I86" t="str">
         <v>SB 354</v>
       </c>
       <c r="J86" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="K86" t="str">
-        <v>SP-First</v>
+        <v>SP-Second</v>
       </c>
       <c r="L86">
         <v>65</v>
       </c>
       <c r="M86" t="str">
-        <v>Artificial Intelligence</v>
+        <v>System Administration: Cloud Services</v>
       </c>
       <c r="N86" t="str">
         <v>Shadow-Gold</v>
@@ -11765,28 +11910,28 @@
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B87" t="str">
         <v>CS</v>
       </c>
       <c r="C87" t="str">
-        <v>376-S</v>
+        <v>374-S</v>
       </c>
       <c r="D87" t="str">
-        <v>B-S</v>
+        <v>A-S</v>
       </c>
       <c r="E87" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F87" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G87" t="str">
-        <v>MWF</v>
+        <v>MW</v>
       </c>
       <c r="H87" t="str">
-        <v>11:00:00 - 12:05:00</v>
+        <v>14:45:00 - 15:50:00</v>
       </c>
       <c r="I87" t="str">
         <v>SB 354</v>
@@ -11795,13 +11940,13 @@
         <v>Second</v>
       </c>
       <c r="K87" t="str">
-        <v>SP-Second</v>
+        <v>FA-Second</v>
       </c>
       <c r="L87">
         <v>65</v>
       </c>
       <c r="M87" t="str">
-        <v>Machine Learning</v>
+        <v>High-Performance Computing</v>
       </c>
       <c r="N87" t="str">
         <v>Shadow-Gold</v>
@@ -11818,13 +11963,13 @@
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B88" t="str">
-        <v>DATA</v>
+        <v>CS</v>
       </c>
       <c r="C88" t="str">
-        <v>202-S</v>
+        <v>375-S</v>
       </c>
       <c r="D88" t="str">
         <v>A-S</v>
@@ -11839,25 +11984,25 @@
         <v>MWF</v>
       </c>
       <c r="H88" t="str">
-        <v>08:00:00 - 09:05:00</v>
+        <v>11:00:00 - 12:05:00</v>
       </c>
       <c r="I88" t="str">
         <v>SB 354</v>
       </c>
       <c r="J88" t="str">
-        <v>Full</v>
+        <v>First</v>
       </c>
       <c r="K88" t="str">
-        <v>FA-Full</v>
+        <v>SP-First</v>
       </c>
       <c r="L88">
         <v>65</v>
       </c>
       <c r="M88" t="str">
-        <v>Predictive Analytics</v>
+        <v>Artificial Intelligence</v>
       </c>
       <c r="N88" t="str">
-        <v>Shadow-Maroon</v>
+        <v>Shadow-Gold</v>
       </c>
       <c r="O88" t="str">
         <v/>
@@ -11871,13 +12016,13 @@
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B89" t="str">
-        <v>DATA</v>
+        <v>CS</v>
       </c>
       <c r="C89" t="str">
-        <v>202-S</v>
+        <v>376-S</v>
       </c>
       <c r="D89" t="str">
         <v>B-S</v>
@@ -11892,25 +12037,25 @@
         <v>MWF</v>
       </c>
       <c r="H89" t="str">
-        <v>09:15:00 - 10:20:00</v>
+        <v>11:00:00 - 12:05:00</v>
       </c>
       <c r="I89" t="str">
         <v>SB 354</v>
       </c>
       <c r="J89" t="str">
-        <v>Full</v>
+        <v>Second</v>
       </c>
       <c r="K89" t="str">
-        <v>FA-Full</v>
+        <v>SP-Second</v>
       </c>
       <c r="L89">
         <v>65</v>
       </c>
       <c r="M89" t="str">
-        <v>Predictive Analytics</v>
+        <v>Machine Learning</v>
       </c>
       <c r="N89" t="str">
-        <v>Shadow-Maroon</v>
+        <v>Shadow-Gold</v>
       </c>
       <c r="O89" t="str">
         <v/>
@@ -11927,28 +12072,28 @@
         <v>FA</v>
       </c>
       <c r="B90" t="str">
-        <v>CS</v>
+        <v>DATA</v>
       </c>
       <c r="C90" t="str">
-        <v>106</v>
+        <v>202-S</v>
       </c>
       <c r="D90" t="str">
-        <v>A</v>
+        <v>A-S</v>
       </c>
       <c r="E90" t="str">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F90" t="str">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G90" t="str">
         <v>MWF</v>
       </c>
       <c r="H90" t="str">
-        <v>14:45:00 - 15:50:00</v>
+        <v>08:00:00 - 09:05:00</v>
       </c>
       <c r="I90" t="str">
-        <v>SB 372</v>
+        <v>SB 354</v>
       </c>
       <c r="J90" t="str">
         <v>Full</v>
@@ -11960,10 +12105,10 @@
         <v>65</v>
       </c>
       <c r="M90" t="str">
-        <v>Intro to Computing</v>
+        <v>Predictive Analytics</v>
       </c>
       <c r="N90" t="str">
-        <v>Staff</v>
+        <v>Shadow-Maroon</v>
       </c>
       <c r="O90" t="str">
         <v/>
@@ -11980,28 +12125,28 @@
         <v>FA</v>
       </c>
       <c r="B91" t="str">
-        <v>CS</v>
+        <v>DATA</v>
       </c>
       <c r="C91" t="str">
-        <v>106L</v>
+        <v>202-S</v>
       </c>
       <c r="D91" t="str">
-        <v>A</v>
+        <v>B-S</v>
       </c>
       <c r="E91" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F91" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G91" t="str">
-        <v>R</v>
+        <v>MWF</v>
       </c>
       <c r="H91" t="str">
-        <v>10:20:00 - 12:00:00</v>
+        <v>09:15:00 - 10:20:00</v>
       </c>
       <c r="I91" t="str">
-        <v>SB 372</v>
+        <v>SB 354</v>
       </c>
       <c r="J91" t="str">
         <v>Full</v>
@@ -12010,13 +12155,13 @@
         <v>FA-Full</v>
       </c>
       <c r="L91">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="M91" t="str">
-        <v>Intro to Computing Lab</v>
+        <v>Predictive Analytics</v>
       </c>
       <c r="N91" t="str">
-        <v>Staff</v>
+        <v>Shadow-Maroon</v>
       </c>
       <c r="O91" t="str">
         <v/>
@@ -12030,19 +12175,19 @@
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B92" t="str">
         <v>CS</v>
       </c>
       <c r="C92" t="str">
-        <v>326</v>
+        <v>106</v>
       </c>
       <c r="D92" t="str">
         <v>A</v>
       </c>
       <c r="E92" t="str">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="str">
         <v>4</v>
@@ -12051,31 +12196,31 @@
         <v>MWF</v>
       </c>
       <c r="H92" t="str">
-        <v>13:30:00 - 14:35:00</v>
+        <v>14:45:00 - 15:50:00</v>
       </c>
       <c r="I92" t="str">
-        <v>SB 301</v>
+        <v>SB 372</v>
       </c>
       <c r="J92" t="str">
         <v>Full</v>
       </c>
       <c r="K92" t="str">
-        <v>SP-Full</v>
+        <v>FA-Full</v>
       </c>
       <c r="L92">
         <v>65</v>
       </c>
       <c r="M92" t="str">
-        <v>Embedded Systems and the Internet of Things</v>
+        <v>Intro to Computing</v>
       </c>
       <c r="N92" t="str">
-        <v>Derek C Schuurman</v>
+        <v>Staff</v>
       </c>
       <c r="O92" t="str">
         <v/>
       </c>
       <c r="P92" t="str">
-        <v>In-Person</v>
+        <v/>
       </c>
       <c r="Q92" t="str">
         <v/>
@@ -12089,25 +12234,25 @@
         <v>CS</v>
       </c>
       <c r="C93" t="str">
-        <v>396</v>
+        <v>106L</v>
       </c>
       <c r="D93" t="str">
         <v>A</v>
       </c>
       <c r="E93" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="str">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="G93" t="str">
-        <v>T</v>
+        <v>R</v>
       </c>
       <c r="H93" t="str">
-        <v>19:00:00 - 19:50:00</v>
+        <v>10:20:00 - 12:00:00</v>
       </c>
       <c r="I93" t="str">
-        <v>SB 382</v>
+        <v>SB 372</v>
       </c>
       <c r="J93" t="str">
         <v>Full</v>
@@ -12116,10 +12261,10 @@
         <v>FA-Full</v>
       </c>
       <c r="L93">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="M93" t="str">
-        <v>Senior Project in Computing I</v>
+        <v>Intro to Computing Lab</v>
       </c>
       <c r="N93" t="str">
         <v>Staff</v>
@@ -12136,52 +12281,52 @@
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B94" t="str">
-        <v>DATA</v>
+        <v>CS</v>
       </c>
       <c r="C94" t="str">
-        <v>396</v>
+        <v>326</v>
       </c>
       <c r="D94" t="str">
         <v>A</v>
       </c>
       <c r="E94" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F94" t="str">
-        <v>0.3</v>
+        <v>4</v>
       </c>
       <c r="G94" t="str">
-        <v>T</v>
+        <v>MWF</v>
       </c>
       <c r="H94" t="str">
-        <v>19:00:00 - 19:50:00</v>
+        <v>13:30:00 - 14:35:00</v>
       </c>
       <c r="I94" t="str">
-        <v>SB 382</v>
+        <v>SB 301</v>
       </c>
       <c r="J94" t="str">
         <v>Full</v>
       </c>
       <c r="K94" t="str">
-        <v>FA-Full</v>
+        <v>SP-Full</v>
       </c>
       <c r="L94">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="M94" t="str">
-        <v>Senior Project in Data Science</v>
+        <v>Embedded Systems and the Internet of Things</v>
       </c>
       <c r="N94" t="str">
-        <v>Staff</v>
+        <v>Derek C Schuurman</v>
       </c>
       <c r="O94" t="str">
         <v/>
       </c>
       <c r="P94" t="str">
-        <v/>
+        <v>In-Person</v>
       </c>
       <c r="Q94" t="str">
         <v/>
@@ -12189,13 +12334,13 @@
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B95" t="str">
         <v>CS</v>
       </c>
       <c r="C95" t="str">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D95" t="str">
         <v>A</v>
@@ -12219,13 +12364,13 @@
         <v>Full</v>
       </c>
       <c r="K95" t="str">
-        <v>SP-Full</v>
+        <v>FA-Full</v>
       </c>
       <c r="L95">
         <v>50</v>
       </c>
       <c r="M95" t="str">
-        <v>Senior Project in Computing II</v>
+        <v>Senior Project in Computing I</v>
       </c>
       <c r="N95" t="str">
         <v>Staff</v>
@@ -12242,13 +12387,13 @@
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B96" t="str">
         <v>DATA</v>
       </c>
       <c r="C96" t="str">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D96" t="str">
         <v>A</v>
@@ -12272,13 +12417,13 @@
         <v>Full</v>
       </c>
       <c r="K96" t="str">
-        <v>SP-Full</v>
+        <v>FA-Full</v>
       </c>
       <c r="L96">
         <v>50</v>
       </c>
       <c r="M96" t="str">
-        <v>Senior Project in Data Science II</v>
+        <v>Senior Project in Data Science</v>
       </c>
       <c r="N96" t="str">
         <v>Staff</v>
@@ -12293,9 +12438,115 @@
         <v/>
       </c>
     </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>SP</v>
+      </c>
+      <c r="B97" t="str">
+        <v>CS</v>
+      </c>
+      <c r="C97" t="str">
+        <v>398</v>
+      </c>
+      <c r="D97" t="str">
+        <v>A</v>
+      </c>
+      <c r="E97" t="str">
+        <v>2</v>
+      </c>
+      <c r="F97" t="str">
+        <v>0.3</v>
+      </c>
+      <c r="G97" t="str">
+        <v>T</v>
+      </c>
+      <c r="H97" t="str">
+        <v>19:00:00 - 19:50:00</v>
+      </c>
+      <c r="I97" t="str">
+        <v>SB 382</v>
+      </c>
+      <c r="J97" t="str">
+        <v>Full</v>
+      </c>
+      <c r="K97" t="str">
+        <v>SP-Full</v>
+      </c>
+      <c r="L97">
+        <v>50</v>
+      </c>
+      <c r="M97" t="str">
+        <v>Senior Project in Computing II</v>
+      </c>
+      <c r="N97" t="str">
+        <v>Staff</v>
+      </c>
+      <c r="O97" t="str">
+        <v/>
+      </c>
+      <c r="P97" t="str">
+        <v/>
+      </c>
+      <c r="Q97" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>SP</v>
+      </c>
+      <c r="B98" t="str">
+        <v>DATA</v>
+      </c>
+      <c r="C98" t="str">
+        <v>398</v>
+      </c>
+      <c r="D98" t="str">
+        <v>A</v>
+      </c>
+      <c r="E98" t="str">
+        <v>2</v>
+      </c>
+      <c r="F98" t="str">
+        <v>0.3</v>
+      </c>
+      <c r="G98" t="str">
+        <v>T</v>
+      </c>
+      <c r="H98" t="str">
+        <v>19:00:00 - 19:50:00</v>
+      </c>
+      <c r="I98" t="str">
+        <v>SB 382</v>
+      </c>
+      <c r="J98" t="str">
+        <v>Full</v>
+      </c>
+      <c r="K98" t="str">
+        <v>SP-Full</v>
+      </c>
+      <c r="L98">
+        <v>50</v>
+      </c>
+      <c r="M98" t="str">
+        <v>Senior Project in Data Science II</v>
+      </c>
+      <c r="N98" t="str">
+        <v>Staff</v>
+      </c>
+      <c r="O98" t="str">
+        <v/>
+      </c>
+      <c r="P98" t="str">
+        <v/>
+      </c>
+      <c r="Q98" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Q96"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Q98"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -12314,7 +12565,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2025-04-03 16:38:07</v>
+        <v>2025-04-07 14:29:36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved HNRS251 to alternate years
</commit_message>
<xml_diff>
--- a/data/schedule_2026.xlsx
+++ b/data/schedule_2026.xlsx
@@ -971,7 +971,7 @@
         <v/>
       </c>
       <c r="D9" t="str">
-        <v/>
+        <v>Full</v>
       </c>
       <c r="E9" t="str">
         <v/>
@@ -1039,7 +1039,7 @@
         <v/>
       </c>
       <c r="D10" t="str">
-        <v/>
+        <v>Full</v>
       </c>
       <c r="E10" t="str">
         <v/>
@@ -1107,7 +1107,7 @@
         <v/>
       </c>
       <c r="D11" t="str">
-        <v/>
+        <v>Full</v>
       </c>
       <c r="E11" t="str">
         <v/>
@@ -1175,7 +1175,7 @@
         <v/>
       </c>
       <c r="D12" t="str">
-        <v/>
+        <v>Full</v>
       </c>
       <c r="E12" t="str">
         <v/>
@@ -3944,7 +3944,7 @@
         <v>FA</v>
       </c>
       <c r="D51" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="E51" t="str">
         <v>CS</v>
@@ -3953,7 +3953,7 @@
         <v>300</v>
       </c>
       <c r="G51" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="H51" t="str">
         <v>Staff</v>
@@ -4015,7 +4015,7 @@
         <v>FA</v>
       </c>
       <c r="D52" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="E52" t="str">
         <v>CS</v>
@@ -4024,10 +4024,10 @@
         <v>300</v>
       </c>
       <c r="G52" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="H52" t="str">
-        <v>Staff</v>
+        <v>Eric Araujo</v>
       </c>
       <c r="I52" t="str">
         <v>2</v>
@@ -6138,7 +6138,7 @@
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>Computer Science</v>
+        <v>Shadow</v>
       </c>
       <c r="B82" t="str">
         <v/>
@@ -6147,49 +6147,49 @@
         <v>FA</v>
       </c>
       <c r="D82" t="str">
-        <v>Full</v>
+        <v>First</v>
       </c>
       <c r="E82" t="str">
-        <v>HNRS</v>
+        <v>CS</v>
       </c>
       <c r="F82" t="str">
-        <v>251</v>
+        <v>300-S</v>
       </c>
       <c r="G82" t="str">
-        <v>A</v>
+        <v>A-S</v>
       </c>
       <c r="H82" t="str">
-        <v>Eric Araujo</v>
+        <v>Shadow-Gold</v>
       </c>
       <c r="I82" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J82" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K82" t="str">
         <v/>
       </c>
       <c r="L82" t="str">
-        <v>TR</v>
+        <v>MWF</v>
       </c>
       <c r="M82" t="str">
-        <v>14:10:00</v>
+        <v>11:00:00</v>
       </c>
       <c r="N82">
         <v>65</v>
       </c>
       <c r="O82" t="str">
-        <v>HL 406C</v>
+        <v>SB 354</v>
       </c>
       <c r="P82" t="str">
-        <v>Agent Modeling</v>
+        <v>Applied Machine Learning</v>
       </c>
       <c r="Q82" t="str">
         <v/>
       </c>
       <c r="R82" t="str">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="S82" t="str">
         <v/>
@@ -6215,10 +6215,10 @@
         <v/>
       </c>
       <c r="C83" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D83" t="str">
-        <v>First</v>
+        <v>Full</v>
       </c>
       <c r="E83" t="str">
         <v>CS</v>
@@ -6245,7 +6245,7 @@
         <v>MWF</v>
       </c>
       <c r="M83" t="str">
-        <v>11:00:00</v>
+        <v>12:15:00</v>
       </c>
       <c r="N83">
         <v>65</v>
@@ -6286,10 +6286,10 @@
         <v/>
       </c>
       <c r="C84" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D84" t="str">
-        <v>Full</v>
+        <v>Second</v>
       </c>
       <c r="E84" t="str">
         <v>CS</v>
@@ -6298,7 +6298,7 @@
         <v>300-S</v>
       </c>
       <c r="G84" t="str">
-        <v>A-S</v>
+        <v>B-S</v>
       </c>
       <c r="H84" t="str">
         <v>Shadow-Gold</v>
@@ -6316,7 +6316,7 @@
         <v>MWF</v>
       </c>
       <c r="M84" t="str">
-        <v>12:15:00</v>
+        <v>11:00:00</v>
       </c>
       <c r="N84">
         <v>65</v>
@@ -6357,19 +6357,19 @@
         <v/>
       </c>
       <c r="C85" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D85" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="E85" t="str">
         <v>CS</v>
       </c>
       <c r="F85" t="str">
-        <v>300-S</v>
+        <v>338-S</v>
       </c>
       <c r="G85" t="str">
-        <v>B-S</v>
+        <v>A-S</v>
       </c>
       <c r="H85" t="str">
         <v>Shadow-Gold</v>
@@ -6387,7 +6387,7 @@
         <v>MWF</v>
       </c>
       <c r="M85" t="str">
-        <v>11:00:00</v>
+        <v>08:00:00</v>
       </c>
       <c r="N85">
         <v>65</v>
@@ -6396,7 +6396,7 @@
         <v>SB 354</v>
       </c>
       <c r="P85" t="str">
-        <v>Applied Machine Learning</v>
+        <v>System Administration: Infrastructure</v>
       </c>
       <c r="Q85" t="str">
         <v/>
@@ -6431,13 +6431,13 @@
         <v>SP</v>
       </c>
       <c r="D86" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="E86" t="str">
         <v>CS</v>
       </c>
       <c r="F86" t="str">
-        <v>338-S</v>
+        <v>339-S</v>
       </c>
       <c r="G86" t="str">
         <v>A-S</v>
@@ -6467,7 +6467,7 @@
         <v>SB 354</v>
       </c>
       <c r="P86" t="str">
-        <v>System Administration: Infrastructure</v>
+        <v>System Administration: Cloud Services</v>
       </c>
       <c r="Q86" t="str">
         <v/>
@@ -6499,7 +6499,7 @@
         <v/>
       </c>
       <c r="C87" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D87" t="str">
         <v>Second</v>
@@ -6508,7 +6508,7 @@
         <v>CS</v>
       </c>
       <c r="F87" t="str">
-        <v>339-S</v>
+        <v>374-S</v>
       </c>
       <c r="G87" t="str">
         <v>A-S</v>
@@ -6517,19 +6517,19 @@
         <v>Shadow-Gold</v>
       </c>
       <c r="I87" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J87" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K87" t="str">
         <v/>
       </c>
       <c r="L87" t="str">
-        <v>MWF</v>
+        <v>MW</v>
       </c>
       <c r="M87" t="str">
-        <v>08:00:00</v>
+        <v>14:45:00</v>
       </c>
       <c r="N87">
         <v>65</v>
@@ -6538,7 +6538,7 @@
         <v>SB 354</v>
       </c>
       <c r="P87" t="str">
-        <v>System Administration: Cloud Services</v>
+        <v>High-Performance Computing</v>
       </c>
       <c r="Q87" t="str">
         <v/>
@@ -6570,16 +6570,16 @@
         <v/>
       </c>
       <c r="C88" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D88" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="E88" t="str">
         <v>CS</v>
       </c>
       <c r="F88" t="str">
-        <v>374-S</v>
+        <v>375-S</v>
       </c>
       <c r="G88" t="str">
         <v>A-S</v>
@@ -6588,19 +6588,19 @@
         <v>Shadow-Gold</v>
       </c>
       <c r="I88" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J88" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K88" t="str">
         <v/>
       </c>
       <c r="L88" t="str">
-        <v>MW</v>
+        <v>MWF</v>
       </c>
       <c r="M88" t="str">
-        <v>14:45:00</v>
+        <v>11:00:00</v>
       </c>
       <c r="N88">
         <v>65</v>
@@ -6609,7 +6609,7 @@
         <v>SB 354</v>
       </c>
       <c r="P88" t="str">
-        <v>High-Performance Computing</v>
+        <v>Artificial Intelligence</v>
       </c>
       <c r="Q88" t="str">
         <v/>
@@ -6644,16 +6644,16 @@
         <v>SP</v>
       </c>
       <c r="D89" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="E89" t="str">
         <v>CS</v>
       </c>
       <c r="F89" t="str">
-        <v>375-S</v>
+        <v>376-S</v>
       </c>
       <c r="G89" t="str">
-        <v>A-S</v>
+        <v>B-S</v>
       </c>
       <c r="H89" t="str">
         <v>Shadow-Gold</v>
@@ -6680,7 +6680,7 @@
         <v>SB 354</v>
       </c>
       <c r="P89" t="str">
-        <v>Artificial Intelligence</v>
+        <v>Machine Learning</v>
       </c>
       <c r="Q89" t="str">
         <v/>
@@ -6712,22 +6712,22 @@
         <v/>
       </c>
       <c r="C90" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D90" t="str">
-        <v>Second</v>
+        <v>Full</v>
       </c>
       <c r="E90" t="str">
-        <v>CS</v>
+        <v>DATA</v>
       </c>
       <c r="F90" t="str">
-        <v>376-S</v>
+        <v>202-S</v>
       </c>
       <c r="G90" t="str">
-        <v>B-S</v>
+        <v>A-S</v>
       </c>
       <c r="H90" t="str">
-        <v>Shadow-Gold</v>
+        <v>Shadow-Maroon</v>
       </c>
       <c r="I90" t="str">
         <v>0</v>
@@ -6742,7 +6742,7 @@
         <v>MWF</v>
       </c>
       <c r="M90" t="str">
-        <v>11:00:00</v>
+        <v>08:00:00</v>
       </c>
       <c r="N90">
         <v>65</v>
@@ -6751,13 +6751,13 @@
         <v>SB 354</v>
       </c>
       <c r="P90" t="str">
-        <v>Machine Learning</v>
+        <v>Predictive Analytics</v>
       </c>
       <c r="Q90" t="str">
         <v/>
       </c>
       <c r="R90" t="str">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="S90" t="str">
         <v/>
@@ -6795,7 +6795,7 @@
         <v>202-S</v>
       </c>
       <c r="G91" t="str">
-        <v>A-S</v>
+        <v>B-S</v>
       </c>
       <c r="H91" t="str">
         <v>Shadow-Maroon</v>
@@ -6813,7 +6813,7 @@
         <v>MWF</v>
       </c>
       <c r="M91" t="str">
-        <v>08:00:00</v>
+        <v>09:15:00</v>
       </c>
       <c r="N91">
         <v>65</v>
@@ -6848,7 +6848,7 @@
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>Shadow</v>
+        <v>Computer Science</v>
       </c>
       <c r="B92" t="str">
         <v/>
@@ -6860,22 +6860,22 @@
         <v>Full</v>
       </c>
       <c r="E92" t="str">
-        <v>DATA</v>
+        <v>CS</v>
       </c>
       <c r="F92" t="str">
-        <v>202-S</v>
+        <v>106</v>
       </c>
       <c r="G92" t="str">
-        <v>B-S</v>
+        <v>A</v>
       </c>
       <c r="H92" t="str">
-        <v>Shadow-Maroon</v>
+        <v>Staff</v>
       </c>
       <c r="I92" t="str">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J92" t="str">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K92" t="str">
         <v/>
@@ -6884,22 +6884,22 @@
         <v>MWF</v>
       </c>
       <c r="M92" t="str">
-        <v>09:15:00</v>
+        <v>14:45:00</v>
       </c>
       <c r="N92">
         <v>65</v>
       </c>
       <c r="O92" t="str">
-        <v>SB 354</v>
+        <v>SB 372</v>
       </c>
       <c r="P92" t="str">
-        <v>Predictive Analytics</v>
+        <v>Intro to Computing</v>
       </c>
       <c r="Q92" t="str">
         <v/>
       </c>
       <c r="R92" t="str">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="S92" t="str">
         <v/>
@@ -6934,7 +6934,7 @@
         <v>CS</v>
       </c>
       <c r="F93" t="str">
-        <v>106</v>
+        <v>106L</v>
       </c>
       <c r="G93" t="str">
         <v>A</v>
@@ -6943,28 +6943,28 @@
         <v>Staff</v>
       </c>
       <c r="I93" t="str">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J93" t="str">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K93" t="str">
         <v/>
       </c>
       <c r="L93" t="str">
-        <v>MWF</v>
+        <v>R</v>
       </c>
       <c r="M93" t="str">
-        <v>14:45:00</v>
+        <v>10:20:00</v>
       </c>
       <c r="N93">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="O93" t="str">
         <v>SB 372</v>
       </c>
       <c r="P93" t="str">
-        <v>Intro to Computing</v>
+        <v>Intro to Computing Lab</v>
       </c>
       <c r="Q93" t="str">
         <v/>
@@ -6996,7 +6996,7 @@
         <v/>
       </c>
       <c r="C94" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D94" t="str">
         <v>Full</v>
@@ -7005,49 +7005,49 @@
         <v>CS</v>
       </c>
       <c r="F94" t="str">
-        <v>106L</v>
+        <v>326</v>
       </c>
       <c r="G94" t="str">
         <v>A</v>
       </c>
       <c r="H94" t="str">
-        <v>Staff</v>
+        <v>Derek C Schuurman</v>
       </c>
       <c r="I94" t="str">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J94" t="str">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K94" t="str">
         <v/>
       </c>
       <c r="L94" t="str">
-        <v>R</v>
+        <v>MWF</v>
       </c>
       <c r="M94" t="str">
-        <v>10:20:00</v>
+        <v>13:30:00</v>
       </c>
       <c r="N94">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="O94" t="str">
-        <v>SB 372</v>
+        <v>SB 301</v>
       </c>
       <c r="P94" t="str">
-        <v>Intro to Computing Lab</v>
+        <v>Embedded Systems and the Internet of Things</v>
       </c>
       <c r="Q94" t="str">
         <v/>
       </c>
       <c r="R94" t="str">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="S94" t="str">
         <v/>
       </c>
       <c r="T94" t="str">
-        <v/>
+        <v>In-Person</v>
       </c>
       <c r="U94" t="str">
         <v/>
@@ -7067,7 +7067,7 @@
         <v/>
       </c>
       <c r="C95" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D95" t="str">
         <v>Full</v>
@@ -7076,37 +7076,37 @@
         <v>CS</v>
       </c>
       <c r="F95" t="str">
-        <v>326</v>
+        <v>396</v>
       </c>
       <c r="G95" t="str">
         <v>A</v>
       </c>
       <c r="H95" t="str">
-        <v>Derek C Schuurman</v>
+        <v>Staff</v>
       </c>
       <c r="I95" t="str">
-        <v>4</v>
+        <v>0.3</v>
       </c>
       <c r="J95" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K95" t="str">
         <v/>
       </c>
       <c r="L95" t="str">
-        <v>MWF</v>
+        <v>T</v>
       </c>
       <c r="M95" t="str">
-        <v>13:30:00</v>
+        <v>19:00:00</v>
       </c>
       <c r="N95">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="O95" t="str">
-        <v>SB 301</v>
+        <v>SB 382</v>
       </c>
       <c r="P95" t="str">
-        <v>Embedded Systems and the Internet of Things</v>
+        <v>Senior Project in Computing I</v>
       </c>
       <c r="Q95" t="str">
         <v/>
@@ -7118,7 +7118,7 @@
         <v/>
       </c>
       <c r="T95" t="str">
-        <v>In-Person</v>
+        <v/>
       </c>
       <c r="U95" t="str">
         <v/>
@@ -7144,7 +7144,7 @@
         <v>Full</v>
       </c>
       <c r="E96" t="str">
-        <v>CS</v>
+        <v>DATA</v>
       </c>
       <c r="F96" t="str">
         <v>396</v>
@@ -7177,7 +7177,7 @@
         <v>SB 382</v>
       </c>
       <c r="P96" t="str">
-        <v>Senior Project in Computing I</v>
+        <v>Senior Project in Data Science</v>
       </c>
       <c r="Q96" t="str">
         <v/>
@@ -7209,16 +7209,16 @@
         <v/>
       </c>
       <c r="C97" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D97" t="str">
         <v>Full</v>
       </c>
       <c r="E97" t="str">
-        <v>DATA</v>
+        <v>CS</v>
       </c>
       <c r="F97" t="str">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="G97" t="str">
         <v>A</v>
@@ -7248,7 +7248,7 @@
         <v>SB 382</v>
       </c>
       <c r="P97" t="str">
-        <v>Senior Project in Data Science</v>
+        <v>Senior Project in Computing II</v>
       </c>
       <c r="Q97" t="str">
         <v/>
@@ -7286,7 +7286,7 @@
         <v>Full</v>
       </c>
       <c r="E98" t="str">
-        <v>CS</v>
+        <v>DATA</v>
       </c>
       <c r="F98" t="str">
         <v>398</v>
@@ -7319,7 +7319,7 @@
         <v>SB 382</v>
       </c>
       <c r="P98" t="str">
-        <v>Senior Project in Computing II</v>
+        <v>Senior Project in Data Science II</v>
       </c>
       <c r="Q98" t="str">
         <v/>
@@ -7351,25 +7351,25 @@
         <v/>
       </c>
       <c r="C99" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D99" t="str">
         <v>Full</v>
       </c>
       <c r="E99" t="str">
-        <v>DATA</v>
+        <v>HNRS</v>
       </c>
       <c r="F99" t="str">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="G99" t="str">
         <v>A</v>
       </c>
       <c r="H99" t="str">
-        <v>Staff</v>
+        <v>Staff-2027</v>
       </c>
       <c r="I99" t="str">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="J99" t="str">
         <v>2</v>
@@ -7378,25 +7378,25 @@
         <v/>
       </c>
       <c r="L99" t="str">
-        <v>T</v>
+        <v>TR</v>
       </c>
       <c r="M99" t="str">
-        <v>19:00:00</v>
+        <v>14:10:00</v>
       </c>
       <c r="N99">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="O99" t="str">
-        <v>SB 382</v>
+        <v>HL 406C</v>
       </c>
       <c r="P99" t="str">
-        <v>Senior Project in Data Science II</v>
+        <v>Agent Modeling</v>
       </c>
       <c r="Q99" t="str">
         <v/>
       </c>
       <c r="R99" t="str">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="S99" t="str">
         <v/>
@@ -7869,7 +7869,10 @@
         <v/>
       </c>
       <c r="J9" t="str">
-        <v/>
+        <v>Full</v>
+      </c>
+      <c r="K9" t="str">
+        <v>-Full</v>
       </c>
       <c r="L9" t="str">
         <v/>
@@ -7916,7 +7919,10 @@
         <v/>
       </c>
       <c r="J10" t="str">
-        <v/>
+        <v>Full</v>
+      </c>
+      <c r="K10" t="str">
+        <v>-Full</v>
       </c>
       <c r="L10" t="str">
         <v/>
@@ -7963,7 +7969,10 @@
         <v/>
       </c>
       <c r="J11" t="str">
-        <v/>
+        <v>Full</v>
+      </c>
+      <c r="K11" t="str">
+        <v>-Full</v>
       </c>
       <c r="L11" t="str">
         <v/>
@@ -8010,7 +8019,10 @@
         <v/>
       </c>
       <c r="J12" t="str">
-        <v/>
+        <v>Full</v>
+      </c>
+      <c r="K12" t="str">
+        <v>-Full</v>
       </c>
       <c r="L12" t="str">
         <v/>
@@ -10056,7 +10068,7 @@
         <v>300</v>
       </c>
       <c r="D51" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="E51" t="str">
         <v>2</v>
@@ -10074,10 +10086,10 @@
         <v>SB 382</v>
       </c>
       <c r="J51" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="K51" t="str">
-        <v>FA-First</v>
+        <v>FA-Second</v>
       </c>
       <c r="L51">
         <v>65</v>
@@ -10109,7 +10121,7 @@
         <v>300</v>
       </c>
       <c r="D52" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="E52" t="str">
         <v>2</v>
@@ -10127,10 +10139,10 @@
         <v>SB 382</v>
       </c>
       <c r="J52" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="K52" t="str">
-        <v>FA-Second</v>
+        <v>FA-First</v>
       </c>
       <c r="L52">
         <v>65</v>
@@ -10139,7 +10151,7 @@
         <v>Applied Machine Learning</v>
       </c>
       <c r="N52" t="str">
-        <v>Staff</v>
+        <v>Eric Araujo</v>
       </c>
       <c r="O52" t="str">
         <v/>
@@ -11695,43 +11707,43 @@
         <v>FA</v>
       </c>
       <c r="B82" t="str">
-        <v>HNRS</v>
+        <v>CS</v>
       </c>
       <c r="C82" t="str">
-        <v>251</v>
+        <v>300-S</v>
       </c>
       <c r="D82" t="str">
-        <v>A</v>
+        <v>A-S</v>
       </c>
       <c r="E82" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F82" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G82" t="str">
-        <v>TR</v>
+        <v>MWF</v>
       </c>
       <c r="H82" t="str">
-        <v>14:10:00 - 15:15:00</v>
+        <v>11:00:00 - 12:05:00</v>
       </c>
       <c r="I82" t="str">
-        <v>HL 406C</v>
+        <v>SB 354</v>
       </c>
       <c r="J82" t="str">
-        <v>Full</v>
+        <v>First</v>
       </c>
       <c r="K82" t="str">
-        <v>FA-Full</v>
+        <v>FA-First</v>
       </c>
       <c r="L82">
         <v>65</v>
       </c>
       <c r="M82" t="str">
-        <v>Agent Modeling</v>
+        <v>Applied Machine Learning</v>
       </c>
       <c r="N82" t="str">
-        <v>Eric Araujo</v>
+        <v>Shadow-Gold</v>
       </c>
       <c r="O82" t="str">
         <v/>
@@ -11745,7 +11757,7 @@
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B83" t="str">
         <v>CS</v>
@@ -11766,16 +11778,16 @@
         <v>MWF</v>
       </c>
       <c r="H83" t="str">
-        <v>11:00:00 - 12:05:00</v>
+        <v>12:15:00 - 13:20:00</v>
       </c>
       <c r="I83" t="str">
         <v>SB 354</v>
       </c>
       <c r="J83" t="str">
-        <v>First</v>
+        <v>Full</v>
       </c>
       <c r="K83" t="str">
-        <v>FA-First</v>
+        <v>SP-Full</v>
       </c>
       <c r="L83">
         <v>65</v>
@@ -11798,7 +11810,7 @@
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B84" t="str">
         <v>CS</v>
@@ -11807,7 +11819,7 @@
         <v>300-S</v>
       </c>
       <c r="D84" t="str">
-        <v>A-S</v>
+        <v>B-S</v>
       </c>
       <c r="E84" t="str">
         <v>0</v>
@@ -11819,16 +11831,16 @@
         <v>MWF</v>
       </c>
       <c r="H84" t="str">
-        <v>12:15:00 - 13:20:00</v>
+        <v>11:00:00 - 12:05:00</v>
       </c>
       <c r="I84" t="str">
         <v>SB 354</v>
       </c>
       <c r="J84" t="str">
-        <v>Full</v>
+        <v>Second</v>
       </c>
       <c r="K84" t="str">
-        <v>SP-Full</v>
+        <v>FA-Second</v>
       </c>
       <c r="L84">
         <v>65</v>
@@ -11851,16 +11863,16 @@
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B85" t="str">
         <v>CS</v>
       </c>
       <c r="C85" t="str">
-        <v>300-S</v>
+        <v>338-S</v>
       </c>
       <c r="D85" t="str">
-        <v>B-S</v>
+        <v>A-S</v>
       </c>
       <c r="E85" t="str">
         <v>0</v>
@@ -11872,22 +11884,22 @@
         <v>MWF</v>
       </c>
       <c r="H85" t="str">
-        <v>11:00:00 - 12:05:00</v>
+        <v>08:00:00 - 09:05:00</v>
       </c>
       <c r="I85" t="str">
         <v>SB 354</v>
       </c>
       <c r="J85" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="K85" t="str">
-        <v>FA-Second</v>
+        <v>SP-First</v>
       </c>
       <c r="L85">
         <v>65</v>
       </c>
       <c r="M85" t="str">
-        <v>Applied Machine Learning</v>
+        <v>System Administration: Infrastructure</v>
       </c>
       <c r="N85" t="str">
         <v>Shadow-Gold</v>
@@ -11910,7 +11922,7 @@
         <v>CS</v>
       </c>
       <c r="C86" t="str">
-        <v>338-S</v>
+        <v>339-S</v>
       </c>
       <c r="D86" t="str">
         <v>A-S</v>
@@ -11931,16 +11943,16 @@
         <v>SB 354</v>
       </c>
       <c r="J86" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="K86" t="str">
-        <v>SP-First</v>
+        <v>SP-Second</v>
       </c>
       <c r="L86">
         <v>65</v>
       </c>
       <c r="M86" t="str">
-        <v>System Administration: Infrastructure</v>
+        <v>System Administration: Cloud Services</v>
       </c>
       <c r="N86" t="str">
         <v>Shadow-Gold</v>
@@ -11957,28 +11969,28 @@
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B87" t="str">
         <v>CS</v>
       </c>
       <c r="C87" t="str">
-        <v>339-S</v>
+        <v>374-S</v>
       </c>
       <c r="D87" t="str">
         <v>A-S</v>
       </c>
       <c r="E87" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F87" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G87" t="str">
-        <v>MWF</v>
+        <v>MW</v>
       </c>
       <c r="H87" t="str">
-        <v>08:00:00 - 09:05:00</v>
+        <v>14:45:00 - 15:50:00</v>
       </c>
       <c r="I87" t="str">
         <v>SB 354</v>
@@ -11987,13 +11999,13 @@
         <v>Second</v>
       </c>
       <c r="K87" t="str">
-        <v>SP-Second</v>
+        <v>FA-Second</v>
       </c>
       <c r="L87">
         <v>65</v>
       </c>
       <c r="M87" t="str">
-        <v>System Administration: Cloud Services</v>
+        <v>High-Performance Computing</v>
       </c>
       <c r="N87" t="str">
         <v>Shadow-Gold</v>
@@ -12010,43 +12022,43 @@
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B88" t="str">
         <v>CS</v>
       </c>
       <c r="C88" t="str">
-        <v>374-S</v>
+        <v>375-S</v>
       </c>
       <c r="D88" t="str">
         <v>A-S</v>
       </c>
       <c r="E88" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F88" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G88" t="str">
-        <v>MW</v>
+        <v>MWF</v>
       </c>
       <c r="H88" t="str">
-        <v>14:45:00 - 15:50:00</v>
+        <v>11:00:00 - 12:05:00</v>
       </c>
       <c r="I88" t="str">
         <v>SB 354</v>
       </c>
       <c r="J88" t="str">
-        <v>Second</v>
+        <v>First</v>
       </c>
       <c r="K88" t="str">
-        <v>FA-Second</v>
+        <v>SP-First</v>
       </c>
       <c r="L88">
         <v>65</v>
       </c>
       <c r="M88" t="str">
-        <v>High-Performance Computing</v>
+        <v>Artificial Intelligence</v>
       </c>
       <c r="N88" t="str">
         <v>Shadow-Gold</v>
@@ -12069,10 +12081,10 @@
         <v>CS</v>
       </c>
       <c r="C89" t="str">
-        <v>375-S</v>
+        <v>376-S</v>
       </c>
       <c r="D89" t="str">
-        <v>A-S</v>
+        <v>B-S</v>
       </c>
       <c r="E89" t="str">
         <v>0</v>
@@ -12090,16 +12102,16 @@
         <v>SB 354</v>
       </c>
       <c r="J89" t="str">
-        <v>First</v>
+        <v>Second</v>
       </c>
       <c r="K89" t="str">
-        <v>SP-First</v>
+        <v>SP-Second</v>
       </c>
       <c r="L89">
         <v>65</v>
       </c>
       <c r="M89" t="str">
-        <v>Artificial Intelligence</v>
+        <v>Machine Learning</v>
       </c>
       <c r="N89" t="str">
         <v>Shadow-Gold</v>
@@ -12116,16 +12128,16 @@
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B90" t="str">
-        <v>CS</v>
+        <v>DATA</v>
       </c>
       <c r="C90" t="str">
-        <v>376-S</v>
+        <v>202-S</v>
       </c>
       <c r="D90" t="str">
-        <v>B-S</v>
+        <v>A-S</v>
       </c>
       <c r="E90" t="str">
         <v>0</v>
@@ -12137,25 +12149,25 @@
         <v>MWF</v>
       </c>
       <c r="H90" t="str">
-        <v>11:00:00 - 12:05:00</v>
+        <v>08:00:00 - 09:05:00</v>
       </c>
       <c r="I90" t="str">
         <v>SB 354</v>
       </c>
       <c r="J90" t="str">
-        <v>Second</v>
+        <v>Full</v>
       </c>
       <c r="K90" t="str">
-        <v>SP-Second</v>
+        <v>FA-Full</v>
       </c>
       <c r="L90">
         <v>65</v>
       </c>
       <c r="M90" t="str">
-        <v>Machine Learning</v>
+        <v>Predictive Analytics</v>
       </c>
       <c r="N90" t="str">
-        <v>Shadow-Gold</v>
+        <v>Shadow-Maroon</v>
       </c>
       <c r="O90" t="str">
         <v/>
@@ -12178,7 +12190,7 @@
         <v>202-S</v>
       </c>
       <c r="D91" t="str">
-        <v>A-S</v>
+        <v>B-S</v>
       </c>
       <c r="E91" t="str">
         <v>0</v>
@@ -12190,7 +12202,7 @@
         <v>MWF</v>
       </c>
       <c r="H91" t="str">
-        <v>08:00:00 - 09:05:00</v>
+        <v>09:15:00 - 10:20:00</v>
       </c>
       <c r="I91" t="str">
         <v>SB 354</v>
@@ -12225,28 +12237,28 @@
         <v>FA</v>
       </c>
       <c r="B92" t="str">
-        <v>DATA</v>
+        <v>CS</v>
       </c>
       <c r="C92" t="str">
-        <v>202-S</v>
+        <v>106</v>
       </c>
       <c r="D92" t="str">
-        <v>B-S</v>
+        <v>A</v>
       </c>
       <c r="E92" t="str">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F92" t="str">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G92" t="str">
         <v>MWF</v>
       </c>
       <c r="H92" t="str">
-        <v>09:15:00 - 10:20:00</v>
+        <v>14:45:00 - 15:50:00</v>
       </c>
       <c r="I92" t="str">
-        <v>SB 354</v>
+        <v>SB 372</v>
       </c>
       <c r="J92" t="str">
         <v>Full</v>
@@ -12258,10 +12270,10 @@
         <v>65</v>
       </c>
       <c r="M92" t="str">
-        <v>Predictive Analytics</v>
+        <v>Intro to Computing</v>
       </c>
       <c r="N92" t="str">
-        <v>Shadow-Maroon</v>
+        <v>Staff</v>
       </c>
       <c r="O92" t="str">
         <v/>
@@ -12281,22 +12293,22 @@
         <v>CS</v>
       </c>
       <c r="C93" t="str">
-        <v>106</v>
+        <v>106L</v>
       </c>
       <c r="D93" t="str">
         <v>A</v>
       </c>
       <c r="E93" t="str">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F93" t="str">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G93" t="str">
-        <v>MWF</v>
+        <v>R</v>
       </c>
       <c r="H93" t="str">
-        <v>14:45:00 - 15:50:00</v>
+        <v>10:20:00 - 12:00:00</v>
       </c>
       <c r="I93" t="str">
         <v>SB 372</v>
@@ -12308,10 +12320,10 @@
         <v>FA-Full</v>
       </c>
       <c r="L93">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="M93" t="str">
-        <v>Intro to Computing</v>
+        <v>Intro to Computing Lab</v>
       </c>
       <c r="N93" t="str">
         <v>Staff</v>
@@ -12328,52 +12340,52 @@
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B94" t="str">
         <v>CS</v>
       </c>
       <c r="C94" t="str">
-        <v>106L</v>
+        <v>326</v>
       </c>
       <c r="D94" t="str">
         <v>A</v>
       </c>
       <c r="E94" t="str">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F94" t="str">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G94" t="str">
-        <v>R</v>
+        <v>MWF</v>
       </c>
       <c r="H94" t="str">
-        <v>10:20:00 - 12:00:00</v>
+        <v>13:30:00 - 14:35:00</v>
       </c>
       <c r="I94" t="str">
-        <v>SB 372</v>
+        <v>SB 301</v>
       </c>
       <c r="J94" t="str">
         <v>Full</v>
       </c>
       <c r="K94" t="str">
-        <v>FA-Full</v>
+        <v>SP-Full</v>
       </c>
       <c r="L94">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="M94" t="str">
-        <v>Intro to Computing Lab</v>
+        <v>Embedded Systems and the Internet of Things</v>
       </c>
       <c r="N94" t="str">
-        <v>Staff</v>
+        <v>Derek C Schuurman</v>
       </c>
       <c r="O94" t="str">
         <v/>
       </c>
       <c r="P94" t="str">
-        <v/>
+        <v>In-Person</v>
       </c>
       <c r="Q94" t="str">
         <v/>
@@ -12381,52 +12393,52 @@
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B95" t="str">
         <v>CS</v>
       </c>
       <c r="C95" t="str">
-        <v>326</v>
+        <v>396</v>
       </c>
       <c r="D95" t="str">
         <v>A</v>
       </c>
       <c r="E95" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F95" t="str">
-        <v>4</v>
+        <v>0.3</v>
       </c>
       <c r="G95" t="str">
-        <v>MWF</v>
+        <v>T</v>
       </c>
       <c r="H95" t="str">
-        <v>13:30:00 - 14:35:00</v>
+        <v>19:00:00 - 19:50:00</v>
       </c>
       <c r="I95" t="str">
-        <v>SB 301</v>
+        <v>SB 382</v>
       </c>
       <c r="J95" t="str">
         <v>Full</v>
       </c>
       <c r="K95" t="str">
-        <v>SP-Full</v>
+        <v>FA-Full</v>
       </c>
       <c r="L95">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="M95" t="str">
-        <v>Embedded Systems and the Internet of Things</v>
+        <v>Senior Project in Computing I</v>
       </c>
       <c r="N95" t="str">
-        <v>Derek C Schuurman</v>
+        <v>Staff</v>
       </c>
       <c r="O95" t="str">
         <v/>
       </c>
       <c r="P95" t="str">
-        <v>In-Person</v>
+        <v/>
       </c>
       <c r="Q95" t="str">
         <v/>
@@ -12437,7 +12449,7 @@
         <v>FA</v>
       </c>
       <c r="B96" t="str">
-        <v>CS</v>
+        <v>DATA</v>
       </c>
       <c r="C96" t="str">
         <v>396</v>
@@ -12470,7 +12482,7 @@
         <v>50</v>
       </c>
       <c r="M96" t="str">
-        <v>Senior Project in Computing I</v>
+        <v>Senior Project in Data Science</v>
       </c>
       <c r="N96" t="str">
         <v>Staff</v>
@@ -12487,13 +12499,13 @@
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B97" t="str">
-        <v>DATA</v>
+        <v>CS</v>
       </c>
       <c r="C97" t="str">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D97" t="str">
         <v>A</v>
@@ -12517,13 +12529,13 @@
         <v>Full</v>
       </c>
       <c r="K97" t="str">
-        <v>FA-Full</v>
+        <v>SP-Full</v>
       </c>
       <c r="L97">
         <v>50</v>
       </c>
       <c r="M97" t="str">
-        <v>Senior Project in Data Science</v>
+        <v>Senior Project in Computing II</v>
       </c>
       <c r="N97" t="str">
         <v>Staff</v>
@@ -12543,7 +12555,7 @@
         <v>SP</v>
       </c>
       <c r="B98" t="str">
-        <v>CS</v>
+        <v>DATA</v>
       </c>
       <c r="C98" t="str">
         <v>398</v>
@@ -12576,7 +12588,7 @@
         <v>50</v>
       </c>
       <c r="M98" t="str">
-        <v>Senior Project in Computing II</v>
+        <v>Senior Project in Data Science II</v>
       </c>
       <c r="N98" t="str">
         <v>Staff</v>
@@ -12593,13 +12605,13 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B99" t="str">
-        <v>DATA</v>
+        <v>HNRS</v>
       </c>
       <c r="C99" t="str">
-        <v>398</v>
+        <v>251</v>
       </c>
       <c r="D99" t="str">
         <v>A</v>
@@ -12608,31 +12620,31 @@
         <v>2</v>
       </c>
       <c r="F99" t="str">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="G99" t="str">
-        <v>T</v>
+        <v>TR</v>
       </c>
       <c r="H99" t="str">
-        <v>19:00:00 - 19:50:00</v>
+        <v>14:10:00 - 15:15:00</v>
       </c>
       <c r="I99" t="str">
-        <v>SB 382</v>
+        <v>HL 406C</v>
       </c>
       <c r="J99" t="str">
         <v>Full</v>
       </c>
       <c r="K99" t="str">
-        <v>SP-Full</v>
+        <v>FA-Full</v>
       </c>
       <c r="L99">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="M99" t="str">
-        <v>Senior Project in Data Science II</v>
+        <v>Agent Modeling</v>
       </c>
       <c r="N99" t="str">
-        <v>Staff</v>
+        <v>Staff-2027</v>
       </c>
       <c r="O99" t="str">
         <v/>
@@ -12665,7 +12677,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2025-04-09 13:20:51</v>
+        <v>2025-04-16 12:39:32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed 39X to 0.25 hours
</commit_message>
<xml_diff>
--- a/data/schedule_2026.xlsx
+++ b/data/schedule_2026.xlsx
@@ -7073,19 +7073,19 @@
         <v>Full</v>
       </c>
       <c r="E95" t="str">
-        <v>CS</v>
+        <v>HNRS</v>
       </c>
       <c r="F95" t="str">
-        <v>396</v>
+        <v>251</v>
       </c>
       <c r="G95" t="str">
         <v>A</v>
       </c>
       <c r="H95" t="str">
-        <v>Staff</v>
+        <v>Staff-2027</v>
       </c>
       <c r="I95" t="str">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="J95" t="str">
         <v>2</v>
@@ -7094,25 +7094,25 @@
         <v/>
       </c>
       <c r="L95" t="str">
-        <v>T</v>
+        <v>TR</v>
       </c>
       <c r="M95" t="str">
-        <v>19:00:00</v>
+        <v>14:10:00</v>
       </c>
       <c r="N95">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="O95" t="str">
-        <v>SB 382</v>
+        <v>HL 406C</v>
       </c>
       <c r="P95" t="str">
-        <v>Senior Project in Computing I</v>
+        <v>Agent Modeling</v>
       </c>
       <c r="Q95" t="str">
         <v/>
       </c>
       <c r="R95" t="str">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="S95" t="str">
         <v/>
@@ -7209,7 +7209,7 @@
         <v/>
       </c>
       <c r="C97" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="D97" t="str">
         <v>Full</v>
@@ -7218,7 +7218,7 @@
         <v>CS</v>
       </c>
       <c r="F97" t="str">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G97" t="str">
         <v>A</v>
@@ -7248,7 +7248,7 @@
         <v>SB 382</v>
       </c>
       <c r="P97" t="str">
-        <v>Senior Project in Computing II</v>
+        <v>Senior Project in Computing I</v>
       </c>
       <c r="Q97" t="str">
         <v/>
@@ -7351,25 +7351,25 @@
         <v/>
       </c>
       <c r="C99" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="D99" t="str">
         <v>Full</v>
       </c>
       <c r="E99" t="str">
-        <v>HNRS</v>
+        <v>CS</v>
       </c>
       <c r="F99" t="str">
-        <v>251</v>
+        <v>398</v>
       </c>
       <c r="G99" t="str">
         <v>A</v>
       </c>
       <c r="H99" t="str">
-        <v>Staff-2027</v>
+        <v>Staff</v>
       </c>
       <c r="I99" t="str">
-        <v>2</v>
+        <v>0.3</v>
       </c>
       <c r="J99" t="str">
         <v>2</v>
@@ -7378,25 +7378,25 @@
         <v/>
       </c>
       <c r="L99" t="str">
-        <v>TR</v>
+        <v>T</v>
       </c>
       <c r="M99" t="str">
-        <v>14:10:00</v>
+        <v>19:00:00</v>
       </c>
       <c r="N99">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="O99" t="str">
-        <v>HL 406C</v>
+        <v>SB 382</v>
       </c>
       <c r="P99" t="str">
-        <v>Agent Modeling</v>
+        <v>Senior Project in Computing II</v>
       </c>
       <c r="Q99" t="str">
         <v/>
       </c>
       <c r="R99" t="str">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="S99" t="str">
         <v/>
@@ -12396,10 +12396,10 @@
         <v>FA</v>
       </c>
       <c r="B95" t="str">
-        <v>CS</v>
+        <v>HNRS</v>
       </c>
       <c r="C95" t="str">
-        <v>396</v>
+        <v>251</v>
       </c>
       <c r="D95" t="str">
         <v>A</v>
@@ -12408,16 +12408,16 @@
         <v>2</v>
       </c>
       <c r="F95" t="str">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="G95" t="str">
-        <v>T</v>
+        <v>TR</v>
       </c>
       <c r="H95" t="str">
-        <v>19:00:00 - 19:50:00</v>
+        <v>14:10:00 - 15:15:00</v>
       </c>
       <c r="I95" t="str">
-        <v>SB 382</v>
+        <v>HL 406C</v>
       </c>
       <c r="J95" t="str">
         <v>Full</v>
@@ -12426,13 +12426,13 @@
         <v>FA-Full</v>
       </c>
       <c r="L95">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="M95" t="str">
-        <v>Senior Project in Computing I</v>
+        <v>Agent Modeling</v>
       </c>
       <c r="N95" t="str">
-        <v>Staff</v>
+        <v>Staff-2027</v>
       </c>
       <c r="O95" t="str">
         <v/>
@@ -12499,13 +12499,13 @@
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>SP</v>
+        <v>FA</v>
       </c>
       <c r="B97" t="str">
         <v>CS</v>
       </c>
       <c r="C97" t="str">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D97" t="str">
         <v>A</v>
@@ -12529,13 +12529,13 @@
         <v>Full</v>
       </c>
       <c r="K97" t="str">
-        <v>SP-Full</v>
+        <v>FA-Full</v>
       </c>
       <c r="L97">
         <v>50</v>
       </c>
       <c r="M97" t="str">
-        <v>Senior Project in Computing II</v>
+        <v>Senior Project in Computing I</v>
       </c>
       <c r="N97" t="str">
         <v>Staff</v>
@@ -12605,13 +12605,13 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>FA</v>
+        <v>SP</v>
       </c>
       <c r="B99" t="str">
-        <v>HNRS</v>
+        <v>CS</v>
       </c>
       <c r="C99" t="str">
-        <v>251</v>
+        <v>398</v>
       </c>
       <c r="D99" t="str">
         <v>A</v>
@@ -12620,31 +12620,31 @@
         <v>2</v>
       </c>
       <c r="F99" t="str">
-        <v>2</v>
+        <v>0.3</v>
       </c>
       <c r="G99" t="str">
-        <v>TR</v>
+        <v>T</v>
       </c>
       <c r="H99" t="str">
-        <v>14:10:00 - 15:15:00</v>
+        <v>19:00:00 - 19:50:00</v>
       </c>
       <c r="I99" t="str">
-        <v>HL 406C</v>
+        <v>SB 382</v>
       </c>
       <c r="J99" t="str">
         <v>Full</v>
       </c>
       <c r="K99" t="str">
-        <v>FA-Full</v>
+        <v>SP-Full</v>
       </c>
       <c r="L99">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="M99" t="str">
-        <v>Agent Modeling</v>
+        <v>Senior Project in Computing II</v>
       </c>
       <c r="N99" t="str">
-        <v>Staff-2027</v>
+        <v>Staff</v>
       </c>
       <c r="O99" t="str">
         <v/>
@@ -12677,7 +12677,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2025-04-16 12:39:32</v>
+        <v>2025-04-17 11:54:18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>